<commit_message>
testbed cityofnewyour case 3
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="25460" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5040" yWindow="460" windowWidth="25460" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -755,72 +755,6 @@
     <xf numFmtId="10" fontId="7" fillId="10" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -832,15 +766,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -850,6 +775,81 @@
     <xf numFmtId="43" fontId="11" fillId="10" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="10" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="10" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W26"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18:S18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,70 +1149,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="44" t="s">
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="74" t="s">
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="76"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="46" t="s">
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="48" t="s">
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="46" t="s">
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
     </row>
     <row r="3" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="32" t="s">
@@ -1236,7 +1236,7 @@
       <c r="J3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="41" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="32" t="s">
@@ -1248,7 +1248,7 @@
       <c r="N3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="66" t="s">
+      <c r="O3" s="44" t="s">
         <v>17</v>
       </c>
       <c r="P3" s="32" t="s">
@@ -1260,7 +1260,7 @@
       <c r="R3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="66" t="s">
+      <c r="S3" s="44" t="s">
         <v>17</v>
       </c>
       <c r="T3" s="32" t="s">
@@ -1272,7 +1272,7 @@
       <c r="V3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="66" t="s">
+      <c r="W3" s="44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1280,7 +1280,7 @@
       <c r="B4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="49" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="34"/>
@@ -1294,21 +1294,21 @@
       <c r="L4" s="34"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
-      <c r="O4" s="67"/>
+      <c r="O4" s="45"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="35"/>
       <c r="R4" s="35"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="79"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="54"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="50" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="34"/>
@@ -1322,49 +1322,57 @@
       <c r="L5" s="34"/>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
-      <c r="O5" s="67"/>
+      <c r="O5" s="45"/>
       <c r="P5" s="34"/>
       <c r="Q5" s="35"/>
       <c r="R5" s="35"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="79"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="54"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="34">
+        <v>0.5</v>
+      </c>
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
       <c r="G6" s="36"/>
-      <c r="H6" s="34"/>
+      <c r="H6" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="36"/>
-      <c r="L6" s="34"/>
+      <c r="L6" s="34">
+        <v>1</v>
+      </c>
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="34"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="34">
+        <v>1</v>
+      </c>
       <c r="Q6" s="35"/>
       <c r="R6" s="35"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="79"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="52"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="54"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="50" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="34">
@@ -1394,7 +1402,7 @@
       <c r="L7" s="34">
         <v>1</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="35">
         <v>1</v>
       </c>
       <c r="N7" s="35">
@@ -1406,7 +1414,7 @@
       <c r="P7" s="34">
         <v>1</v>
       </c>
-      <c r="Q7" s="34">
+      <c r="Q7" s="35">
         <v>1</v>
       </c>
       <c r="R7" s="35">
@@ -1415,20 +1423,22 @@
       <c r="S7" s="35">
         <v>1</v>
       </c>
-      <c r="T7" s="77">
+      <c r="T7" s="52">
         <v>260</v>
       </c>
-      <c r="U7" s="78">
+      <c r="U7" s="53">
         <v>987</v>
       </c>
-      <c r="V7" s="78">
+      <c r="V7" s="53">
         <v>300</v>
       </c>
-      <c r="W7" s="79"/>
+      <c r="W7" s="54">
+        <v>879</v>
+      </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
-      <c r="C8" s="72"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="34"/>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
@@ -1440,19 +1450,19 @@
       <c r="L8" s="34"/>
       <c r="M8" s="35"/>
       <c r="N8" s="35"/>
-      <c r="O8" s="67"/>
+      <c r="O8" s="45"/>
       <c r="P8" s="34"/>
       <c r="Q8" s="35"/>
       <c r="R8" s="35"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="79"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="54"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
-      <c r="C9" s="72"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="34"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
@@ -1464,19 +1474,19 @@
       <c r="L9" s="34"/>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
-      <c r="O9" s="67"/>
+      <c r="O9" s="45"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="35"/>
       <c r="R9" s="35"/>
-      <c r="S9" s="67"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="79"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="54"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
-      <c r="C10" s="72"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="34"/>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
@@ -1488,19 +1498,19 @@
       <c r="L10" s="34"/>
       <c r="M10" s="35"/>
       <c r="N10" s="35"/>
-      <c r="O10" s="67"/>
+      <c r="O10" s="45"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="35"/>
       <c r="R10" s="35"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="78"/>
-      <c r="W10" s="79"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="52"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="54"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
-      <c r="C11" s="72"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="34"/>
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
@@ -1512,19 +1522,19 @@
       <c r="L11" s="34"/>
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
-      <c r="O11" s="67"/>
+      <c r="O11" s="45"/>
       <c r="P11" s="34"/>
       <c r="Q11" s="35"/>
       <c r="R11" s="35"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="77"/>
-      <c r="U11" s="78"/>
-      <c r="V11" s="78"/>
-      <c r="W11" s="79"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="54"/>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="73"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="37"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
@@ -1532,24 +1542,24 @@
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
-      <c r="K12" s="64"/>
+      <c r="K12" s="42"/>
       <c r="L12" s="37"/>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
-      <c r="O12" s="68"/>
+      <c r="O12" s="46"/>
       <c r="P12" s="37"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
-      <c r="S12" s="68"/>
-      <c r="T12" s="80"/>
-      <c r="U12" s="81"/>
-      <c r="V12" s="81"/>
-      <c r="W12" s="82"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="56"/>
+      <c r="V12" s="56"/>
+      <c r="W12" s="57"/>
     </row>
     <row r="13" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D13" s="39">
         <f>AVERAGE(D4:D12)</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E13" s="40">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
@@ -1565,7 +1575,7 @@
       </c>
       <c r="H13" s="40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="I13" s="40">
         <f t="shared" si="0"/>
@@ -1575,7 +1585,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K13" s="65">
+      <c r="K13" s="43">
         <f t="shared" si="0"/>
         <v>7.6899999999999996E-2</v>
       </c>
@@ -1591,7 +1601,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O13" s="69">
+      <c r="O13" s="47">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1607,32 +1617,32 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S13" s="69">
+      <c r="S13" s="47">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T13" s="83">
+      <c r="T13" s="58">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
         <v>260</v>
       </c>
-      <c r="U13" s="84">
+      <c r="U13" s="59">
         <f t="shared" si="1"/>
         <v>987</v>
       </c>
-      <c r="V13" s="84">
+      <c r="V13" s="59">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="W13" s="85" t="e">
+      <c r="W13" s="60">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>879</v>
       </c>
     </row>
     <row r="16" spans="2:23" ht="64" x14ac:dyDescent="0.2">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1651,15 +1661,15 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42" t="s">
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
@@ -1680,17 +1690,17 @@
       <c r="H17">
         <v>10</v>
       </c>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42">
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66">
         <v>1711</v>
       </c>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1711,17 +1721,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42">
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66">
         <v>9407</v>
       </c>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -1742,17 +1752,17 @@
       <c r="H19">
         <v>10</v>
       </c>
-      <c r="M19" s="42" t="s">
+      <c r="M19" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42">
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66">
         <v>499302</v>
       </c>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -1773,17 +1783,17 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="M20" s="50" t="s">
+      <c r="M20" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="51" t="s">
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="51"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
@@ -1812,6 +1822,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="M19:O19"/>
@@ -1823,14 +1841,6 @@
     <mergeCell ref="P18:S18"/>
     <mergeCell ref="M18:O18"/>
     <mergeCell ref="M17:O17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P20" r:id="rId1"/>
@@ -1843,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,46 +1869,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="44" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="M2" s="60" t="s">
+      <c r="K2" s="75"/>
+      <c r="M2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="85"/>
+      <c r="O2" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="52"/>
+      <c r="P2" s="75"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57" t="s">
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="59"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
       <c r="J3" s="16" t="s">
         <v>11</v>
       </c>
@@ -2036,14 +2046,30 @@
       <c r="C7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.1429</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
       <c r="M7" s="25"/>
       <c r="N7" s="26"/>
       <c r="O7" s="25"/>
@@ -2066,10 +2092,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>0.98860000000000003</v>
+        <v>0.05</v>
       </c>
       <c r="H8" s="19">
-        <v>0.98860000000000003</v>
+        <v>0.05</v>
       </c>
       <c r="I8" s="6">
         <v>2.63E-2</v>
@@ -2180,23 +2206,23 @@
       </c>
       <c r="G14" s="13">
         <f>AVERAGE(G5:G13)</f>
-        <v>0.98860000000000003</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>0.98860000000000003</v>
+        <v>0.05</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="1"/>
-        <v>2.63E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" ref="J14:K14" si="2">AVERAGE(J5:J13)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="2"/>
-        <v>0.12909999999999999</v>
+        <v>6.4549999999999996E-2</v>
       </c>
       <c r="M14" s="29" t="e">
         <f t="shared" ref="M14:N14" si="3">AVERAGE(M5:M13)</f>

</xml_diff>

<commit_message>
new condition “and” checker
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
   <si>
     <t>th_krm</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>****</t>
+  </si>
+  <si>
+    <t>5_wm</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -681,6 +684,73 @@
     </border>
     <border>
       <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
@@ -702,7 +772,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -732,7 +802,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -768,84 +837,6 @@
     <xf numFmtId="10" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -854,6 +845,89 @@
     <xf numFmtId="43" fontId="7" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="7" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1140,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,130 +1227,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66" t="s">
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="72" t="s">
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="74"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72"/>
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="68" t="s">
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="70" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="68" t="s">
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="44" t="s">
+      <c r="S3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="32" t="s">
+      <c r="T3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="44" t="s">
+      <c r="W3" s="43" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1284,67 +1358,67 @@
       <c r="B4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="34">
-        <v>1</v>
-      </c>
-      <c r="E4" s="90">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35">
-        <v>1</v>
-      </c>
-      <c r="G4" s="35">
-        <v>1</v>
-      </c>
-      <c r="H4" s="60">
+      <c r="D4" s="33">
+        <v>1</v>
+      </c>
+      <c r="E4" s="63">
+        <v>1</v>
+      </c>
+      <c r="F4" s="34">
+        <v>1</v>
+      </c>
+      <c r="G4" s="34">
+        <v>1</v>
+      </c>
+      <c r="H4" s="59">
         <v>0</v>
       </c>
-      <c r="I4" s="90">
-        <v>1</v>
-      </c>
-      <c r="J4" s="35">
-        <v>1</v>
-      </c>
-      <c r="K4" s="36">
-        <v>1</v>
-      </c>
-      <c r="L4" s="60">
+      <c r="I4" s="63">
+        <v>1</v>
+      </c>
+      <c r="J4" s="34">
+        <v>1</v>
+      </c>
+      <c r="K4" s="35">
+        <v>1</v>
+      </c>
+      <c r="L4" s="59">
         <v>0</v>
       </c>
-      <c r="M4" s="90">
-        <v>1</v>
-      </c>
-      <c r="N4" s="35">
-        <v>1</v>
-      </c>
-      <c r="O4" s="45">
-        <v>1</v>
-      </c>
-      <c r="P4" s="60">
+      <c r="M4" s="63">
+        <v>1</v>
+      </c>
+      <c r="N4" s="34">
+        <v>1</v>
+      </c>
+      <c r="O4" s="44">
+        <v>1</v>
+      </c>
+      <c r="P4" s="59">
         <v>0</v>
       </c>
-      <c r="Q4" s="90">
-        <v>1</v>
-      </c>
-      <c r="R4" s="35">
+      <c r="Q4" s="63">
+        <v>1</v>
+      </c>
+      <c r="R4" s="34">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="S4" s="45">
+      <c r="S4" s="44">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="T4" s="51">
+      <c r="T4" s="50">
         <v>211</v>
       </c>
-      <c r="U4" s="94">
+      <c r="U4" s="67">
         <v>479</v>
       </c>
-      <c r="V4" s="52">
+      <c r="V4" s="51">
         <v>448</v>
       </c>
-      <c r="W4" s="53">
+      <c r="W4" s="52">
         <v>475</v>
       </c>
     </row>
@@ -1352,67 +1426,67 @@
       <c r="B5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="34">
-        <v>1</v>
-      </c>
-      <c r="E5" s="90">
+      <c r="D5" s="33">
+        <v>1</v>
+      </c>
+      <c r="E5" s="63">
         <v>0.5</v>
       </c>
-      <c r="F5" s="35">
-        <v>1</v>
-      </c>
-      <c r="G5" s="36">
+      <c r="F5" s="34">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35">
         <v>0.5</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="33">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="I5" s="90">
+      <c r="I5" s="63">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="34">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="35">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="L5" s="34">
-        <v>1</v>
-      </c>
-      <c r="M5" s="90">
-        <v>1</v>
-      </c>
-      <c r="N5" s="35">
-        <v>1</v>
-      </c>
-      <c r="O5" s="45">
-        <v>1</v>
-      </c>
-      <c r="P5" s="34">
+      <c r="L5" s="33">
+        <v>1</v>
+      </c>
+      <c r="M5" s="63">
+        <v>1</v>
+      </c>
+      <c r="N5" s="34">
+        <v>1</v>
+      </c>
+      <c r="O5" s="44">
+        <v>1</v>
+      </c>
+      <c r="P5" s="33">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="Q5" s="90">
+      <c r="Q5" s="63">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="34">
         <v>3.3E-3</v>
       </c>
-      <c r="S5" s="45">
+      <c r="S5" s="44">
         <v>1E-4</v>
       </c>
-      <c r="T5" s="51">
+      <c r="T5" s="50">
         <v>627</v>
       </c>
-      <c r="U5" s="94">
+      <c r="U5" s="67">
         <v>3702</v>
       </c>
-      <c r="V5" s="52">
+      <c r="V5" s="51">
         <v>704</v>
       </c>
-      <c r="W5" s="53">
+      <c r="W5" s="52">
         <v>5129</v>
       </c>
     </row>
@@ -1420,67 +1494,67 @@
       <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="34">
-        <v>1</v>
-      </c>
-      <c r="E6" s="90">
-        <v>1</v>
-      </c>
-      <c r="F6" s="35">
-        <v>1</v>
-      </c>
-      <c r="G6" s="36">
-        <v>1</v>
-      </c>
-      <c r="H6" s="34">
-        <v>1</v>
-      </c>
-      <c r="I6" s="90">
-        <v>1</v>
-      </c>
-      <c r="J6" s="35">
-        <v>1</v>
-      </c>
-      <c r="K6" s="36">
-        <v>1</v>
-      </c>
-      <c r="L6" s="34">
-        <v>1</v>
-      </c>
-      <c r="M6" s="90">
-        <v>1</v>
-      </c>
-      <c r="N6" s="35">
-        <v>1</v>
-      </c>
-      <c r="O6" s="45">
-        <v>1</v>
-      </c>
-      <c r="P6" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="90">
-        <v>1</v>
-      </c>
-      <c r="R6" s="35">
-        <v>1</v>
-      </c>
-      <c r="S6" s="45">
-        <v>1</v>
-      </c>
-      <c r="T6" s="51">
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="63">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1</v>
+      </c>
+      <c r="I6" s="63">
+        <v>1</v>
+      </c>
+      <c r="J6" s="34">
+        <v>1</v>
+      </c>
+      <c r="K6" s="35">
+        <v>1</v>
+      </c>
+      <c r="L6" s="33">
+        <v>1</v>
+      </c>
+      <c r="M6" s="63">
+        <v>1</v>
+      </c>
+      <c r="N6" s="34">
+        <v>1</v>
+      </c>
+      <c r="O6" s="44">
+        <v>1</v>
+      </c>
+      <c r="P6" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="63">
+        <v>1</v>
+      </c>
+      <c r="R6" s="34">
+        <v>1</v>
+      </c>
+      <c r="S6" s="44">
+        <v>1</v>
+      </c>
+      <c r="T6" s="50">
         <v>499</v>
       </c>
-      <c r="U6" s="94">
+      <c r="U6" s="67">
         <v>705</v>
       </c>
-      <c r="V6" s="52">
+      <c r="V6" s="51">
         <v>465</v>
       </c>
-      <c r="W6" s="53">
+      <c r="W6" s="52">
         <v>507</v>
       </c>
     </row>
@@ -1488,294 +1562,298 @@
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="34">
-        <v>1</v>
-      </c>
-      <c r="E7" s="90">
-        <v>1</v>
-      </c>
-      <c r="F7" s="35">
-        <v>1</v>
-      </c>
-      <c r="G7" s="35">
-        <v>1</v>
-      </c>
-      <c r="H7" s="34">
-        <v>1</v>
-      </c>
-      <c r="I7" s="90">
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="63">
+        <v>1</v>
+      </c>
+      <c r="F7" s="34">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1</v>
+      </c>
+      <c r="I7" s="63">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J7" s="35">
-        <v>1</v>
-      </c>
-      <c r="K7" s="35">
+      <c r="J7" s="34">
+        <v>1</v>
+      </c>
+      <c r="K7" s="34">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="L7" s="34">
-        <v>1</v>
-      </c>
-      <c r="M7" s="90">
-        <v>1</v>
-      </c>
-      <c r="N7" s="35">
-        <v>1</v>
-      </c>
-      <c r="O7" s="35">
-        <v>1</v>
-      </c>
-      <c r="P7" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="90">
-        <v>1</v>
-      </c>
-      <c r="R7" s="35">
-        <v>1</v>
-      </c>
-      <c r="S7" s="35">
-        <v>1</v>
-      </c>
-      <c r="T7" s="51">
+      <c r="L7" s="33">
+        <v>1</v>
+      </c>
+      <c r="M7" s="63">
+        <v>1</v>
+      </c>
+      <c r="N7" s="34">
+        <v>1</v>
+      </c>
+      <c r="O7" s="34">
+        <v>1</v>
+      </c>
+      <c r="P7" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="63">
+        <v>1</v>
+      </c>
+      <c r="R7" s="34">
+        <v>1</v>
+      </c>
+      <c r="S7" s="34">
+        <v>1</v>
+      </c>
+      <c r="T7" s="50">
         <v>260</v>
       </c>
-      <c r="U7" s="94">
+      <c r="U7" s="67">
         <v>987</v>
       </c>
-      <c r="V7" s="52">
+      <c r="V7" s="51">
         <v>300</v>
       </c>
-      <c r="W7" s="53">
+      <c r="W7" s="52">
         <v>879</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="53"/>
+      <c r="B8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="67"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="52"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="53"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="52"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="51"/>
-      <c r="U10" s="94"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="53"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="52"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="94"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="53"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="52"/>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="91"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="54"/>
-      <c r="U12" s="95"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="56"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="54"/>
+      <c r="W12" s="55"/>
     </row>
     <row r="13" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <f>AVERAGE(D4:D12)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="92">
+      <c r="E13" s="65">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
         <v>0.875</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="39">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="39">
         <f t="shared" si="0"/>
         <v>0.52082499999999998</v>
       </c>
-      <c r="I13" s="92">
+      <c r="I13" s="65">
         <f t="shared" si="0"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="39">
         <f t="shared" si="0"/>
         <v>0.77082499999999998</v>
       </c>
-      <c r="K13" s="43">
+      <c r="K13" s="42">
         <f t="shared" si="0"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="L13" s="39">
+      <c r="L13" s="38">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="M13" s="92">
+      <c r="M13" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="39">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="46">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P13" s="39">
+      <c r="P13" s="38">
         <f t="shared" si="0"/>
         <v>0.50392499999999996</v>
       </c>
-      <c r="Q13" s="92">
+      <c r="Q13" s="65">
         <f t="shared" si="0"/>
         <v>0.75022499999999992</v>
       </c>
-      <c r="R13" s="40">
+      <c r="R13" s="39">
         <f t="shared" si="0"/>
         <v>0.51170000000000004</v>
       </c>
-      <c r="S13" s="47">
+      <c r="S13" s="46">
         <f t="shared" si="0"/>
         <v>0.51090000000000002</v>
       </c>
-      <c r="T13" s="57">
+      <c r="T13" s="56">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
         <v>399.25</v>
       </c>
-      <c r="U13" s="96">
+      <c r="U13" s="69">
         <f t="shared" si="1"/>
         <v>1468.25</v>
       </c>
-      <c r="V13" s="58">
+      <c r="V13" s="57">
         <f t="shared" si="1"/>
         <v>479.25</v>
       </c>
-      <c r="W13" s="59">
+      <c r="W13" s="58">
         <f t="shared" si="1"/>
         <v>1747.5</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="93" t="s">
+      <c r="I14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="93" t="s">
+      <c r="M14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="93" t="s">
+      <c r="Q14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="U14" s="93" t="s">
+      <c r="U14" s="66" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="63"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1794,15 +1872,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="64" t="s">
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="64"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1823,17 +1901,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="64" t="s">
+      <c r="M18" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="64"/>
-      <c r="O18" s="64"/>
-      <c r="P18" s="64">
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75">
         <v>1711</v>
       </c>
-      <c r="Q18" s="64"/>
-      <c r="R18" s="64"/>
-      <c r="S18" s="64"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -1857,17 +1935,17 @@
       <c r="I19" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="64" t="s">
+      <c r="M19" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
-      <c r="P19" s="64">
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="75">
         <v>9407</v>
       </c>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="64"/>
-      <c r="S19" s="64"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -1888,17 +1966,17 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="M20" s="64" t="s">
+      <c r="M20" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="76">
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="79">
         <v>1162725581</v>
       </c>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -1919,17 +1997,17 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="M21" s="75" t="s">
+      <c r="M21" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="77" t="s">
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
-      <c r="S21" s="77"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
@@ -1958,6 +2036,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="M20:O20"/>
@@ -1969,14 +2055,6 @@
     <mergeCell ref="P19:S19"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="M18:O18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P18:S18"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P21" r:id="rId1"/>
@@ -1989,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:V4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2005,46 +2083,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="66" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="M2" s="86" t="s">
+      <c r="K2" s="85"/>
+      <c r="M2" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="88"/>
-      <c r="O2" s="66" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="78"/>
+      <c r="P2" s="85"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83" t="s">
+      <c r="E3" s="88"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="85"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="92"/>
       <c r="J3" s="16" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2141,7 @@
       <c r="P3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="30" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -2119,7 +2197,7 @@
       <c r="N4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="96" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="24" t="s">
@@ -2149,10 +2227,10 @@
       <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="59">
         <v>0</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="60">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -2167,22 +2245,22 @@
       <c r="I5" s="6">
         <v>0.01</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="61">
         <v>0</v>
       </c>
-      <c r="K5" s="62">
+      <c r="K5" s="61">
         <v>0</v>
       </c>
-      <c r="M5" s="90">
-        <v>1</v>
-      </c>
-      <c r="N5" s="90">
-        <v>1</v>
-      </c>
-      <c r="O5" s="90">
-        <v>1</v>
-      </c>
-      <c r="P5" s="90">
+      <c r="M5" s="25">
+        <v>1</v>
+      </c>
+      <c r="N5" s="26">
+        <v>1</v>
+      </c>
+      <c r="O5" s="97">
+        <v>1</v>
+      </c>
+      <c r="P5" s="63">
         <v>1</v>
       </c>
     </row>
@@ -2217,16 +2295,16 @@
       <c r="K6" s="6">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M6" s="90">
+      <c r="M6" s="25">
         <v>0.5</v>
       </c>
-      <c r="N6" s="90">
+      <c r="N6" s="26">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="O6" s="90">
-        <v>1</v>
-      </c>
-      <c r="P6" s="90">
+      <c r="O6" s="97">
+        <v>1</v>
+      </c>
+      <c r="P6" s="63">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
@@ -2237,19 +2315,19 @@
       <c r="C7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="59">
         <v>0</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="60">
         <v>0</v>
       </c>
       <c r="F7" s="6">
         <v>0.25</v>
       </c>
-      <c r="G7" s="60">
+      <c r="G7" s="59">
         <v>0</v>
       </c>
-      <c r="H7" s="61">
+      <c r="H7" s="60">
         <v>0</v>
       </c>
       <c r="I7" s="6">
@@ -2261,16 +2339,16 @@
       <c r="K7" s="6">
         <v>1</v>
       </c>
-      <c r="M7" s="90">
-        <v>1</v>
-      </c>
-      <c r="N7" s="90">
-        <v>1</v>
-      </c>
-      <c r="O7" s="90">
-        <v>1</v>
-      </c>
-      <c r="P7" s="90">
+      <c r="M7" s="25">
+        <v>1</v>
+      </c>
+      <c r="N7" s="26">
+        <v>1</v>
+      </c>
+      <c r="O7" s="97">
+        <v>1</v>
+      </c>
+      <c r="P7" s="63">
         <v>1</v>
       </c>
     </row>
@@ -2305,33 +2383,45 @@
       <c r="K8" s="6">
         <v>0.12909999999999999</v>
       </c>
-      <c r="M8" s="90">
-        <v>1</v>
-      </c>
-      <c r="N8" s="90">
+      <c r="M8" s="25">
+        <v>1</v>
+      </c>
+      <c r="N8" s="26">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="O8" s="90">
-        <v>1</v>
-      </c>
-      <c r="P8" s="90">
+      <c r="O8" s="97">
+        <v>1</v>
+      </c>
+      <c r="P8" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="19"/>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.15</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="M9" s="25"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="25"/>
+      <c r="O9" s="97"/>
       <c r="P9" s="26"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
@@ -2347,7 +2437,7 @@
       <c r="K10" s="6"/>
       <c r="M10" s="25"/>
       <c r="N10" s="26"/>
-      <c r="O10" s="25"/>
+      <c r="O10" s="97"/>
       <c r="P10" s="26"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
@@ -2363,7 +2453,7 @@
       <c r="K11" s="6"/>
       <c r="M11" s="25"/>
       <c r="N11" s="26"/>
-      <c r="O11" s="25"/>
+      <c r="O11" s="97"/>
       <c r="P11" s="26"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
@@ -2379,7 +2469,7 @@
       <c r="K12" s="6"/>
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="97"/>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2393,19 +2483,19 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="13">
         <f>AVERAGE(D5:D13)</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E14" s="21">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="0"/>
@@ -2413,11 +2503,11 @@
       </c>
       <c r="G14" s="13">
         <f>AVERAGE(G5:G13)</f>
-        <v>0.13750000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>6.25E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="1"/>
@@ -2431,18 +2521,18 @@
         <f t="shared" si="2"/>
         <v>0.28237499999999999</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="28">
         <f t="shared" ref="M14:N14" si="3">AVERAGE(M5:M13)</f>
         <v>0.875</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="29">
         <f t="shared" si="3"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="O14" s="29">
-        <v>1</v>
-      </c>
-      <c r="P14" s="30">
+      <c r="O14" s="28">
+        <v>1</v>
+      </c>
+      <c r="P14" s="29">
         <v>0.63263333333333327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test 2 query 5_wm
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>th_krm</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>5_wm</t>
+  </si>
+  <si>
+    <t>6_wm</t>
+  </si>
+  <si>
+    <t>7_wm</t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -437,32 +443,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -760,6 +740,21 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -772,7 +767,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -782,82 +777,80 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="9" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="7" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="10" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="10" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="10" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="10" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="10" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="10" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="7" fillId="10" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="7" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="10" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="10" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="10" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="10" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="10" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="10" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="10" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="7" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="7" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="7" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -866,10 +859,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -881,53 +874,54 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1214,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,633 +1221,643 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="83" t="s">
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="70" t="s">
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="72"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="77" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="73" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="77" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="73" t="s">
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="72"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="43" t="s">
+      <c r="S3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="T3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="43" t="s">
+      <c r="W3" s="41" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="33">
-        <v>1</v>
-      </c>
-      <c r="E4" s="63">
-        <v>1</v>
-      </c>
-      <c r="F4" s="34">
-        <v>1</v>
-      </c>
-      <c r="G4" s="34">
-        <v>1</v>
-      </c>
-      <c r="H4" s="59">
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="61">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1</v>
+      </c>
+      <c r="G4" s="32">
+        <v>1</v>
+      </c>
+      <c r="H4" s="57">
         <v>0</v>
       </c>
-      <c r="I4" s="63">
-        <v>1</v>
-      </c>
-      <c r="J4" s="34">
-        <v>1</v>
-      </c>
-      <c r="K4" s="35">
-        <v>1</v>
-      </c>
-      <c r="L4" s="59">
+      <c r="I4" s="61">
+        <v>1</v>
+      </c>
+      <c r="J4" s="32">
+        <v>1</v>
+      </c>
+      <c r="K4" s="33">
+        <v>1</v>
+      </c>
+      <c r="L4" s="57">
         <v>0</v>
       </c>
-      <c r="M4" s="63">
-        <v>1</v>
-      </c>
-      <c r="N4" s="34">
-        <v>1</v>
-      </c>
-      <c r="O4" s="44">
-        <v>1</v>
-      </c>
-      <c r="P4" s="59">
+      <c r="M4" s="61">
+        <v>1</v>
+      </c>
+      <c r="N4" s="32">
+        <v>1</v>
+      </c>
+      <c r="O4" s="42">
+        <v>1</v>
+      </c>
+      <c r="P4" s="57">
         <v>0</v>
       </c>
-      <c r="Q4" s="63">
-        <v>1</v>
-      </c>
-      <c r="R4" s="34">
+      <c r="Q4" s="61">
+        <v>1</v>
+      </c>
+      <c r="R4" s="32">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="S4" s="44">
+      <c r="S4" s="42">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="T4" s="50">
+      <c r="T4" s="48">
         <v>211</v>
       </c>
-      <c r="U4" s="67">
+      <c r="U4" s="65">
         <v>479</v>
       </c>
-      <c r="V4" s="51">
+      <c r="V4" s="49">
         <v>448</v>
       </c>
-      <c r="W4" s="52">
+      <c r="W4" s="50">
         <v>475</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="33">
-        <v>1</v>
-      </c>
-      <c r="E5" s="63">
+      <c r="D5" s="31">
+        <v>1</v>
+      </c>
+      <c r="E5" s="61">
         <v>0.5</v>
       </c>
-      <c r="F5" s="34">
-        <v>1</v>
-      </c>
-      <c r="G5" s="35">
+      <c r="F5" s="32">
+        <v>1</v>
+      </c>
+      <c r="G5" s="33">
         <v>0.5</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="31">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="61">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="32">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="33">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="L5" s="33">
-        <v>1</v>
-      </c>
-      <c r="M5" s="63">
-        <v>1</v>
-      </c>
-      <c r="N5" s="34">
-        <v>1</v>
-      </c>
-      <c r="O5" s="44">
-        <v>1</v>
-      </c>
-      <c r="P5" s="33">
+      <c r="L5" s="31">
+        <v>1</v>
+      </c>
+      <c r="M5" s="61">
+        <v>1</v>
+      </c>
+      <c r="N5" s="32">
+        <v>1</v>
+      </c>
+      <c r="O5" s="42">
+        <v>1</v>
+      </c>
+      <c r="P5" s="31">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="Q5" s="63">
+      <c r="Q5" s="61">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="32">
         <v>3.3E-3</v>
       </c>
-      <c r="S5" s="44">
+      <c r="S5" s="42">
         <v>1E-4</v>
       </c>
-      <c r="T5" s="50">
+      <c r="T5" s="48">
         <v>627</v>
       </c>
-      <c r="U5" s="67">
+      <c r="U5" s="65">
         <v>3702</v>
       </c>
-      <c r="V5" s="51">
+      <c r="V5" s="49">
         <v>704</v>
       </c>
-      <c r="W5" s="52">
+      <c r="W5" s="50">
         <v>5129</v>
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="33">
-        <v>1</v>
-      </c>
-      <c r="E6" s="63">
-        <v>1</v>
-      </c>
-      <c r="F6" s="34">
-        <v>1</v>
-      </c>
-      <c r="G6" s="35">
-        <v>1</v>
-      </c>
-      <c r="H6" s="33">
-        <v>1</v>
-      </c>
-      <c r="I6" s="63">
-        <v>1</v>
-      </c>
-      <c r="J6" s="34">
-        <v>1</v>
-      </c>
-      <c r="K6" s="35">
-        <v>1</v>
-      </c>
-      <c r="L6" s="33">
-        <v>1</v>
-      </c>
-      <c r="M6" s="63">
-        <v>1</v>
-      </c>
-      <c r="N6" s="34">
-        <v>1</v>
-      </c>
-      <c r="O6" s="44">
-        <v>1</v>
-      </c>
-      <c r="P6" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="63">
-        <v>1</v>
-      </c>
-      <c r="R6" s="34">
-        <v>1</v>
-      </c>
-      <c r="S6" s="44">
-        <v>1</v>
-      </c>
-      <c r="T6" s="50">
+      <c r="D6" s="31">
+        <v>1</v>
+      </c>
+      <c r="E6" s="61">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="31">
+        <v>1</v>
+      </c>
+      <c r="I6" s="61">
+        <v>1</v>
+      </c>
+      <c r="J6" s="32">
+        <v>1</v>
+      </c>
+      <c r="K6" s="33">
+        <v>1</v>
+      </c>
+      <c r="L6" s="31">
+        <v>1</v>
+      </c>
+      <c r="M6" s="61">
+        <v>1</v>
+      </c>
+      <c r="N6" s="32">
+        <v>1</v>
+      </c>
+      <c r="O6" s="42">
+        <v>1</v>
+      </c>
+      <c r="P6" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="61">
+        <v>1</v>
+      </c>
+      <c r="R6" s="32">
+        <v>1</v>
+      </c>
+      <c r="S6" s="42">
+        <v>1</v>
+      </c>
+      <c r="T6" s="48">
         <v>499</v>
       </c>
-      <c r="U6" s="67">
+      <c r="U6" s="65">
         <v>705</v>
       </c>
-      <c r="V6" s="51">
+      <c r="V6" s="49">
         <v>465</v>
       </c>
-      <c r="W6" s="52">
+      <c r="W6" s="50">
         <v>507</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="33">
-        <v>1</v>
-      </c>
-      <c r="E7" s="63">
-        <v>1</v>
-      </c>
-      <c r="F7" s="34">
-        <v>1</v>
-      </c>
-      <c r="G7" s="34">
-        <v>1</v>
-      </c>
-      <c r="H7" s="33">
-        <v>1</v>
-      </c>
-      <c r="I7" s="63">
+      <c r="D7" s="31">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61">
+        <v>1</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>1</v>
+      </c>
+      <c r="H7" s="31">
+        <v>1</v>
+      </c>
+      <c r="I7" s="61">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J7" s="34">
-        <v>1</v>
-      </c>
-      <c r="K7" s="34">
+      <c r="J7" s="32">
+        <v>1</v>
+      </c>
+      <c r="K7" s="32">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="L7" s="33">
-        <v>1</v>
-      </c>
-      <c r="M7" s="63">
-        <v>1</v>
-      </c>
-      <c r="N7" s="34">
-        <v>1</v>
-      </c>
-      <c r="O7" s="34">
-        <v>1</v>
-      </c>
-      <c r="P7" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="63">
-        <v>1</v>
-      </c>
-      <c r="R7" s="34">
-        <v>1</v>
-      </c>
-      <c r="S7" s="34">
-        <v>1</v>
-      </c>
-      <c r="T7" s="50">
+      <c r="L7" s="31">
+        <v>1</v>
+      </c>
+      <c r="M7" s="61">
+        <v>1</v>
+      </c>
+      <c r="N7" s="32">
+        <v>1</v>
+      </c>
+      <c r="O7" s="32">
+        <v>1</v>
+      </c>
+      <c r="P7" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="61">
+        <v>1</v>
+      </c>
+      <c r="R7" s="32">
+        <v>1</v>
+      </c>
+      <c r="S7" s="32">
+        <v>1</v>
+      </c>
+      <c r="T7" s="48">
         <v>260</v>
       </c>
-      <c r="U7" s="67">
+      <c r="U7" s="65">
         <v>987</v>
       </c>
-      <c r="V7" s="51">
+      <c r="V7" s="49">
         <v>300</v>
       </c>
-      <c r="W7" s="52">
+      <c r="W7" s="50">
         <v>879</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="67"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="52"/>
+      <c r="D8" s="31">
+        <v>1</v>
+      </c>
+      <c r="E8" s="61"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="31">
+        <v>1</v>
+      </c>
+      <c r="I8" s="61"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="31">
+        <v>1</v>
+      </c>
+      <c r="M8" s="61"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="48">
+        <v>308</v>
+      </c>
+      <c r="U8" s="65"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="50"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="52"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="50"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="50"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="51"/>
-      <c r="W10" s="52"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="50"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="51"/>
-      <c r="W11" s="52"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="65"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="50"/>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="54"/>
-      <c r="W12" s="55"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="53"/>
     </row>
     <row r="13" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="38">
+      <c r="D13" s="36">
         <f>AVERAGE(D4:D12)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="63">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
         <v>0.875</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="37">
         <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
-        <v>0.52082499999999998</v>
-      </c>
-      <c r="I13" s="65">
+        <v>0.61665999999999999</v>
+      </c>
+      <c r="I13" s="63">
         <f t="shared" si="0"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="37">
         <f t="shared" si="0"/>
         <v>0.77082499999999998</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="40">
         <f t="shared" si="0"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="L13" s="38">
+      <c r="L13" s="36">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="M13" s="65">
+        <v>0.8</v>
+      </c>
+      <c r="M13" s="63">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N13" s="39">
+      <c r="N13" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O13" s="46">
+      <c r="O13" s="44">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P13" s="38">
+      <c r="P13" s="36">
         <f t="shared" si="0"/>
-        <v>0.50392499999999996</v>
-      </c>
-      <c r="Q13" s="65">
+        <v>0.60314000000000001</v>
+      </c>
+      <c r="Q13" s="63">
         <f t="shared" si="0"/>
         <v>0.75022499999999992</v>
       </c>
-      <c r="R13" s="39">
+      <c r="R13" s="37">
         <f t="shared" si="0"/>
         <v>0.51170000000000004</v>
       </c>
-      <c r="S13" s="46">
+      <c r="S13" s="44">
         <f t="shared" si="0"/>
         <v>0.51090000000000002</v>
       </c>
-      <c r="T13" s="56">
+      <c r="T13" s="54">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
-        <v>399.25</v>
-      </c>
-      <c r="U13" s="69">
+        <v>381</v>
+      </c>
+      <c r="U13" s="67">
         <f t="shared" si="1"/>
         <v>1468.25</v>
       </c>
-      <c r="V13" s="57">
+      <c r="V13" s="55">
         <f t="shared" si="1"/>
         <v>479.25</v>
       </c>
-      <c r="W13" s="58">
+      <c r="W13" s="56">
         <f t="shared" si="1"/>
         <v>1747.5</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="66" t="s">
+      <c r="I14" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="66" t="s">
+      <c r="M14" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="66" t="s">
+      <c r="Q14" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="U14" s="66" t="s">
+      <c r="U14" s="64" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,15 +1876,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75" t="s">
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="75"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="73"/>
+      <c r="S17" s="73"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1901,17 +1905,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="75" t="s">
+      <c r="M18" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75">
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73">
         <v>1711</v>
       </c>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -1935,17 +1939,17 @@
       <c r="I19" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="75" t="s">
+      <c r="M19" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75">
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73">
         <v>9407</v>
       </c>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73"/>
+      <c r="S19" s="73"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -1966,17 +1970,17 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="M20" s="75" t="s">
+      <c r="M20" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="75"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="79">
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="77">
         <v>1162725581</v>
       </c>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77"/>
+      <c r="S20" s="77"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -1997,17 +2001,17 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="M21" s="76" t="s">
+      <c r="M21" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="76"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="80" t="s">
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="80"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78"/>
+      <c r="S21" s="78"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
@@ -2067,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2083,65 +2087,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="83" t="s">
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="M2" s="93" t="s">
+      <c r="K2" s="83"/>
+      <c r="M2" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="95"/>
-      <c r="O2" s="83" t="s">
+      <c r="N2" s="93"/>
+      <c r="O2" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="85"/>
+      <c r="P2" s="83"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="90" t="s">
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="91"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="16" t="s">
+      <c r="H3" s="89"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="28" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -2161,46 +2165,46 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="99" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="15" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="96" t="s">
+      <c r="O4" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="2"/>
@@ -2221,16 +2225,16 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="57">
         <v>0</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="58">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -2239,42 +2243,42 @@
       <c r="G5" s="5">
         <v>0</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="17">
         <v>0</v>
       </c>
       <c r="I5" s="6">
         <v>0.01</v>
       </c>
-      <c r="J5" s="61">
+      <c r="J5" s="59">
         <v>0</v>
       </c>
-      <c r="K5" s="61">
+      <c r="K5" s="59">
         <v>0</v>
       </c>
-      <c r="M5" s="25">
-        <v>1</v>
-      </c>
-      <c r="N5" s="26">
-        <v>1</v>
-      </c>
-      <c r="O5" s="97">
-        <v>1</v>
-      </c>
-      <c r="P5" s="63">
+      <c r="M5" s="23">
+        <v>1</v>
+      </c>
+      <c r="N5" s="24">
+        <v>1</v>
+      </c>
+      <c r="O5" s="95">
+        <v>1</v>
+      </c>
+      <c r="P5" s="61">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="46" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>1</v>
       </c>
       <c r="F6" s="6">
@@ -2283,7 +2287,7 @@
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="17">
         <v>0.2</v>
       </c>
       <c r="I6" s="6">
@@ -2295,39 +2299,39 @@
       <c r="K6" s="6">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="23">
         <v>0.5</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="24">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="O6" s="97">
-        <v>1</v>
-      </c>
-      <c r="P6" s="63">
+      <c r="O6" s="95">
+        <v>1</v>
+      </c>
+      <c r="P6" s="61">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="57">
         <v>0</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="58">
         <v>0</v>
       </c>
       <c r="F7" s="6">
         <v>0.25</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="57">
         <v>0</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="58">
         <v>0</v>
       </c>
       <c r="I7" s="6">
@@ -2339,30 +2343,30 @@
       <c r="K7" s="6">
         <v>1</v>
       </c>
-      <c r="M7" s="25">
-        <v>1</v>
-      </c>
-      <c r="N7" s="26">
-        <v>1</v>
-      </c>
-      <c r="O7" s="97">
-        <v>1</v>
-      </c>
-      <c r="P7" s="63">
+      <c r="M7" s="23">
+        <v>1</v>
+      </c>
+      <c r="N7" s="24">
+        <v>1</v>
+      </c>
+      <c r="O7" s="95">
+        <v>1</v>
+      </c>
+      <c r="P7" s="61">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="46" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>1</v>
       </c>
       <c r="F8" s="6">
@@ -2371,7 +2375,7 @@
       <c r="G8" s="5">
         <v>0.05</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="17">
         <v>0.05</v>
       </c>
       <c r="I8" s="6">
@@ -2383,165 +2387,181 @@
       <c r="K8" s="6">
         <v>0.12909999999999999</v>
       </c>
-      <c r="M8" s="25">
-        <v>1</v>
-      </c>
-      <c r="N8" s="26">
+      <c r="M8" s="23">
+        <v>1</v>
+      </c>
+      <c r="N8" s="24">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="O8" s="97">
-        <v>1</v>
-      </c>
-      <c r="P8" s="63">
+      <c r="O8" s="95">
+        <v>1</v>
+      </c>
+      <c r="P8" s="61">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="46" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="19">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6"/>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="59">
+        <v>0</v>
+      </c>
       <c r="G9" s="5">
         <v>0.15</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <v>0.15</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="26"/>
+      <c r="I9" s="59">
+        <v>0</v>
+      </c>
+      <c r="J9" s="59">
+        <v>0</v>
+      </c>
+      <c r="K9" s="59">
+        <v>0</v>
+      </c>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="95"/>
+      <c r="P9" s="24"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="19"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="97"/>
-      <c r="P10" s="26"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="19"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="97"/>
-      <c r="P11" s="26"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="24"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="19"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="97"/>
-      <c r="P12" s="26"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="24"/>
     </row>
     <row r="13" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="27"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="96"/>
+      <c r="P13" s="25"/>
     </row>
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <f>AVERAGE(D5:D13)</f>
         <v>0.6</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="19">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
         <v>0.6</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>0.8125</v>
-      </c>
-      <c r="G14" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="G14" s="11">
         <f>AVERAGE(G5:G13)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="19">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
         <v>0.08</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="12">
         <f t="shared" si="1"/>
-        <v>0.27575</v>
-      </c>
-      <c r="J14" s="14">
+        <v>0.22059999999999999</v>
+      </c>
+      <c r="J14" s="12">
         <f t="shared" ref="J14:K14" si="2">AVERAGE(J5:J13)</f>
-        <v>0.75</v>
-      </c>
-      <c r="K14" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="K14" s="12">
         <f t="shared" si="2"/>
-        <v>0.28237499999999999</v>
-      </c>
-      <c r="M14" s="28">
+        <v>0.22589999999999999</v>
+      </c>
+      <c r="M14" s="26">
         <f t="shared" ref="M14:N14" si="3">AVERAGE(M5:M13)</f>
         <v>0.875</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="27">
         <f t="shared" si="3"/>
         <v>0.52100000000000013</v>
       </c>
-      <c r="O14" s="28">
-        <v>1</v>
-      </c>
-      <c r="P14" s="29">
+      <c r="O14" s="26">
+        <v>1</v>
+      </c>
+      <c r="P14" s="27">
         <v>0.63263333333333327</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="13"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="15"/>
+      <c r="E18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
test 3 - query 5_wn
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -1209,7 +1209,7 @@
   <dimension ref="B1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1630,31 +1630,41 @@
       <c r="D8" s="31">
         <v>1</v>
       </c>
-      <c r="E8" s="61"/>
+      <c r="E8" s="61">
+        <v>1</v>
+      </c>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
       <c r="H8" s="31">
         <v>1</v>
       </c>
-      <c r="I8" s="61"/>
+      <c r="I8" s="61">
+        <v>1</v>
+      </c>
       <c r="J8" s="32"/>
       <c r="K8" s="33"/>
       <c r="L8" s="31">
         <v>1</v>
       </c>
-      <c r="M8" s="61"/>
+      <c r="M8" s="61">
+        <v>1</v>
+      </c>
       <c r="N8" s="32"/>
       <c r="O8" s="42"/>
       <c r="P8" s="31">
         <v>1</v>
       </c>
-      <c r="Q8" s="61"/>
+      <c r="Q8" s="61">
+        <v>1</v>
+      </c>
       <c r="R8" s="32"/>
       <c r="S8" s="42"/>
       <c r="T8" s="48">
         <v>308</v>
       </c>
-      <c r="U8" s="65"/>
+      <c r="U8" s="65">
+        <v>343</v>
+      </c>
       <c r="V8" s="49"/>
       <c r="W8" s="50"/>
     </row>
@@ -1761,7 +1771,7 @@
       </c>
       <c r="E13" s="63">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="F13" s="37">
         <f t="shared" si="0"/>
@@ -1777,7 +1787,7 @@
       </c>
       <c r="I13" s="63">
         <f t="shared" si="0"/>
-        <v>0.52100000000000013</v>
+        <v>0.61680000000000013</v>
       </c>
       <c r="J13" s="37">
         <f t="shared" si="0"/>
@@ -1809,7 +1819,7 @@
       </c>
       <c r="Q13" s="63">
         <f t="shared" si="0"/>
-        <v>0.75022499999999992</v>
+        <v>0.80017999999999989</v>
       </c>
       <c r="R13" s="37">
         <f t="shared" si="0"/>
@@ -1825,7 +1835,7 @@
       </c>
       <c r="U13" s="67">
         <f t="shared" si="1"/>
-        <v>1468.25</v>
+        <v>1243.2</v>
       </c>
       <c r="V13" s="55">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
test 3 - query 5_wm
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
   <si>
     <t>th_krm</t>
   </si>
@@ -1209,7 +1209,7 @@
   <dimension ref="B1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1633,7 +1633,9 @@
       <c r="E8" s="61">
         <v>1</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="32">
+        <v>1</v>
+      </c>
       <c r="G8" s="33"/>
       <c r="H8" s="31">
         <v>1</v>
@@ -1641,7 +1643,9 @@
       <c r="I8" s="61">
         <v>1</v>
       </c>
-      <c r="J8" s="32"/>
+      <c r="J8" s="32">
+        <v>1</v>
+      </c>
       <c r="K8" s="33"/>
       <c r="L8" s="31">
         <v>1</v>
@@ -1649,7 +1653,9 @@
       <c r="M8" s="61">
         <v>1</v>
       </c>
-      <c r="N8" s="32"/>
+      <c r="N8" s="32">
+        <v>1</v>
+      </c>
       <c r="O8" s="42"/>
       <c r="P8" s="31">
         <v>1</v>
@@ -1657,7 +1663,9 @@
       <c r="Q8" s="61">
         <v>1</v>
       </c>
-      <c r="R8" s="32"/>
+      <c r="R8" s="32">
+        <v>1</v>
+      </c>
       <c r="S8" s="42"/>
       <c r="T8" s="48">
         <v>308</v>
@@ -1665,12 +1673,18 @@
       <c r="U8" s="65">
         <v>343</v>
       </c>
-      <c r="V8" s="49"/>
+      <c r="V8" s="49">
+        <v>347</v>
+      </c>
       <c r="W8" s="50"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="8"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D9" s="31"/>
       <c r="E9" s="61"/>
       <c r="F9" s="32"/>
@@ -1693,8 +1707,12 @@
       <c r="W9" s="50"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="8"/>
-      <c r="C10" s="46"/>
+      <c r="B10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="31"/>
       <c r="E10" s="61"/>
       <c r="F10" s="32"/>
@@ -1791,7 +1809,7 @@
       </c>
       <c r="J13" s="37">
         <f t="shared" si="0"/>
-        <v>0.77082499999999998</v>
+        <v>0.81665999999999994</v>
       </c>
       <c r="K13" s="40">
         <f t="shared" si="0"/>
@@ -1823,7 +1841,7 @@
       </c>
       <c r="R13" s="37">
         <f t="shared" si="0"/>
-        <v>0.51170000000000004</v>
+        <v>0.60936000000000001</v>
       </c>
       <c r="S13" s="44">
         <f t="shared" si="0"/>
@@ -1839,7 +1857,7 @@
       </c>
       <c r="V13" s="55">
         <f t="shared" si="1"/>
-        <v>479.25</v>
+        <v>452.8</v>
       </c>
       <c r="W13" s="56">
         <f t="shared" si="1"/>
@@ -2081,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="B5:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test 4 - query 5_wn
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -767,7 +767,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -797,7 +797,6 @@
     <xf numFmtId="10" fontId="7" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1208,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,130 +1220,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="81" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="68" t="s">
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="69"/>
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="75" t="s">
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="71" t="s">
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="75" t="s">
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="71" t="s">
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="41" t="s">
+      <c r="O3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="29" t="s">
+      <c r="P3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="41" t="s">
+      <c r="S3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="T3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="30" t="s">
+      <c r="U3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="41" t="s">
+      <c r="W3" s="40" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1352,67 +1351,67 @@
       <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="31">
-        <v>1</v>
-      </c>
-      <c r="E4" s="61">
-        <v>1</v>
-      </c>
-      <c r="F4" s="32">
-        <v>1</v>
-      </c>
-      <c r="G4" s="32">
-        <v>1</v>
-      </c>
-      <c r="H4" s="57">
+      <c r="D4" s="30">
+        <v>1</v>
+      </c>
+      <c r="E4" s="60">
+        <v>1</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+      <c r="G4" s="31">
+        <v>1</v>
+      </c>
+      <c r="H4" s="56">
         <v>0</v>
       </c>
-      <c r="I4" s="61">
-        <v>1</v>
-      </c>
-      <c r="J4" s="32">
-        <v>1</v>
-      </c>
-      <c r="K4" s="33">
-        <v>1</v>
-      </c>
-      <c r="L4" s="57">
+      <c r="I4" s="60">
+        <v>1</v>
+      </c>
+      <c r="J4" s="31">
+        <v>1</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1</v>
+      </c>
+      <c r="L4" s="56">
         <v>0</v>
       </c>
-      <c r="M4" s="61">
-        <v>1</v>
-      </c>
-      <c r="N4" s="32">
-        <v>1</v>
-      </c>
-      <c r="O4" s="42">
-        <v>1</v>
-      </c>
-      <c r="P4" s="57">
+      <c r="M4" s="60">
+        <v>1</v>
+      </c>
+      <c r="N4" s="31">
+        <v>1</v>
+      </c>
+      <c r="O4" s="41">
+        <v>1</v>
+      </c>
+      <c r="P4" s="56">
         <v>0</v>
       </c>
-      <c r="Q4" s="61">
-        <v>1</v>
-      </c>
-      <c r="R4" s="32">
+      <c r="Q4" s="60">
+        <v>1</v>
+      </c>
+      <c r="R4" s="31">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="S4" s="42">
+      <c r="S4" s="41">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="T4" s="48">
+      <c r="T4" s="47">
         <v>211</v>
       </c>
-      <c r="U4" s="65">
+      <c r="U4" s="64">
         <v>479</v>
       </c>
-      <c r="V4" s="49">
+      <c r="V4" s="48">
         <v>448</v>
       </c>
-      <c r="W4" s="50">
+      <c r="W4" s="49">
         <v>475</v>
       </c>
     </row>
@@ -1420,67 +1419,67 @@
       <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="31">
-        <v>1</v>
-      </c>
-      <c r="E5" s="61">
+      <c r="D5" s="30">
+        <v>1</v>
+      </c>
+      <c r="E5" s="60">
         <v>0.5</v>
       </c>
-      <c r="F5" s="32">
-        <v>1</v>
-      </c>
-      <c r="G5" s="33">
+      <c r="F5" s="31">
+        <v>1</v>
+      </c>
+      <c r="G5" s="32">
         <v>0.5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="60">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="31">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="32">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="L5" s="31">
-        <v>1</v>
-      </c>
-      <c r="M5" s="61">
-        <v>1</v>
-      </c>
-      <c r="N5" s="32">
-        <v>1</v>
-      </c>
-      <c r="O5" s="42">
-        <v>1</v>
-      </c>
-      <c r="P5" s="31">
+      <c r="L5" s="30">
+        <v>1</v>
+      </c>
+      <c r="M5" s="60">
+        <v>1</v>
+      </c>
+      <c r="N5" s="31">
+        <v>1</v>
+      </c>
+      <c r="O5" s="41">
+        <v>1</v>
+      </c>
+      <c r="P5" s="30">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="Q5" s="61">
+      <c r="Q5" s="60">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="31">
         <v>3.3E-3</v>
       </c>
-      <c r="S5" s="42">
+      <c r="S5" s="41">
         <v>1E-4</v>
       </c>
-      <c r="T5" s="48">
+      <c r="T5" s="47">
         <v>627</v>
       </c>
-      <c r="U5" s="65">
+      <c r="U5" s="64">
         <v>3702</v>
       </c>
-      <c r="V5" s="49">
+      <c r="V5" s="48">
         <v>704</v>
       </c>
-      <c r="W5" s="50">
+      <c r="W5" s="49">
         <v>5129</v>
       </c>
     </row>
@@ -1488,67 +1487,67 @@
       <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="31">
-        <v>1</v>
-      </c>
-      <c r="E6" s="61">
-        <v>1</v>
-      </c>
-      <c r="F6" s="32">
-        <v>1</v>
-      </c>
-      <c r="G6" s="33">
-        <v>1</v>
-      </c>
-      <c r="H6" s="31">
-        <v>1</v>
-      </c>
-      <c r="I6" s="61">
-        <v>1</v>
-      </c>
-      <c r="J6" s="32">
-        <v>1</v>
-      </c>
-      <c r="K6" s="33">
-        <v>1</v>
-      </c>
-      <c r="L6" s="31">
-        <v>1</v>
-      </c>
-      <c r="M6" s="61">
-        <v>1</v>
-      </c>
-      <c r="N6" s="32">
-        <v>1</v>
-      </c>
-      <c r="O6" s="42">
-        <v>1</v>
-      </c>
-      <c r="P6" s="31">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="61">
-        <v>1</v>
-      </c>
-      <c r="R6" s="32">
-        <v>1</v>
-      </c>
-      <c r="S6" s="42">
-        <v>1</v>
-      </c>
-      <c r="T6" s="48">
+      <c r="D6" s="30">
+        <v>1</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1</v>
+      </c>
+      <c r="I6" s="60">
+        <v>1</v>
+      </c>
+      <c r="J6" s="31">
+        <v>1</v>
+      </c>
+      <c r="K6" s="32">
+        <v>1</v>
+      </c>
+      <c r="L6" s="30">
+        <v>1</v>
+      </c>
+      <c r="M6" s="60">
+        <v>1</v>
+      </c>
+      <c r="N6" s="31">
+        <v>1</v>
+      </c>
+      <c r="O6" s="41">
+        <v>1</v>
+      </c>
+      <c r="P6" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="60">
+        <v>1</v>
+      </c>
+      <c r="R6" s="31">
+        <v>1</v>
+      </c>
+      <c r="S6" s="41">
+        <v>1</v>
+      </c>
+      <c r="T6" s="47">
         <v>499</v>
       </c>
-      <c r="U6" s="65">
+      <c r="U6" s="64">
         <v>705</v>
       </c>
-      <c r="V6" s="49">
+      <c r="V6" s="48">
         <v>465</v>
       </c>
-      <c r="W6" s="50">
+      <c r="W6" s="49">
         <v>507</v>
       </c>
     </row>
@@ -1556,67 +1555,67 @@
       <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="61">
-        <v>1</v>
-      </c>
-      <c r="F7" s="32">
-        <v>1</v>
-      </c>
-      <c r="G7" s="32">
-        <v>1</v>
-      </c>
-      <c r="H7" s="31">
-        <v>1</v>
-      </c>
-      <c r="I7" s="61">
+      <c r="D7" s="30">
+        <v>1</v>
+      </c>
+      <c r="E7" s="60">
+        <v>1</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="31">
+        <v>1</v>
+      </c>
+      <c r="H7" s="30">
+        <v>1</v>
+      </c>
+      <c r="I7" s="60">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J7" s="32">
-        <v>1</v>
-      </c>
-      <c r="K7" s="32">
+      <c r="J7" s="31">
+        <v>1</v>
+      </c>
+      <c r="K7" s="31">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="L7" s="31">
-        <v>1</v>
-      </c>
-      <c r="M7" s="61">
-        <v>1</v>
-      </c>
-      <c r="N7" s="32">
-        <v>1</v>
-      </c>
-      <c r="O7" s="32">
-        <v>1</v>
-      </c>
-      <c r="P7" s="31">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="61">
-        <v>1</v>
-      </c>
-      <c r="R7" s="32">
-        <v>1</v>
-      </c>
-      <c r="S7" s="32">
-        <v>1</v>
-      </c>
-      <c r="T7" s="48">
+      <c r="L7" s="30">
+        <v>1</v>
+      </c>
+      <c r="M7" s="60">
+        <v>1</v>
+      </c>
+      <c r="N7" s="31">
+        <v>1</v>
+      </c>
+      <c r="O7" s="31">
+        <v>1</v>
+      </c>
+      <c r="P7" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="60">
+        <v>1</v>
+      </c>
+      <c r="R7" s="31">
+        <v>1</v>
+      </c>
+      <c r="S7" s="31">
+        <v>1</v>
+      </c>
+      <c r="T7" s="47">
         <v>260</v>
       </c>
-      <c r="U7" s="65">
+      <c r="U7" s="64">
         <v>987</v>
       </c>
-      <c r="V7" s="49">
+      <c r="V7" s="48">
         <v>300</v>
       </c>
-      <c r="W7" s="50">
+      <c r="W7" s="49">
         <v>879</v>
       </c>
     </row>
@@ -1624,268 +1623,278 @@
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="31">
-        <v>1</v>
-      </c>
-      <c r="E8" s="61">
-        <v>1</v>
-      </c>
-      <c r="F8" s="32">
-        <v>1</v>
-      </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="31">
-        <v>1</v>
-      </c>
-      <c r="I8" s="61">
-        <v>1</v>
-      </c>
-      <c r="J8" s="32">
-        <v>1</v>
-      </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="31">
-        <v>1</v>
-      </c>
-      <c r="M8" s="61">
-        <v>1</v>
-      </c>
-      <c r="N8" s="32">
-        <v>1</v>
-      </c>
-      <c r="O8" s="42"/>
-      <c r="P8" s="31">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="61">
-        <v>1</v>
-      </c>
-      <c r="R8" s="32">
-        <v>1</v>
-      </c>
-      <c r="S8" s="42"/>
-      <c r="T8" s="48">
+      <c r="D8" s="30">
+        <v>1</v>
+      </c>
+      <c r="E8" s="60">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="32">
+        <v>1</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1</v>
+      </c>
+      <c r="I8" s="60">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1</v>
+      </c>
+      <c r="K8" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="30">
+        <v>1</v>
+      </c>
+      <c r="M8" s="60">
+        <v>1</v>
+      </c>
+      <c r="N8" s="31">
+        <v>1</v>
+      </c>
+      <c r="O8" s="41">
+        <v>1</v>
+      </c>
+      <c r="P8" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="60">
+        <v>1</v>
+      </c>
+      <c r="R8" s="31">
+        <v>1</v>
+      </c>
+      <c r="S8" s="41">
+        <v>1</v>
+      </c>
+      <c r="T8" s="47">
         <v>308</v>
       </c>
-      <c r="U8" s="65">
+      <c r="U8" s="64">
         <v>343</v>
       </c>
-      <c r="V8" s="49">
+      <c r="V8" s="48">
         <v>347</v>
       </c>
-      <c r="W8" s="50"/>
+      <c r="W8" s="49">
+        <v>3085</v>
+      </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="65"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="50"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="49"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="50"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="49"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="49"/>
-      <c r="W11" s="50"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="49"/>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="53"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="52"/>
     </row>
     <row r="13" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="36">
+      <c r="D13" s="35">
         <f>AVERAGE(D4:D12)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="62">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
         <v>0.9</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="36">
         <f t="shared" si="0"/>
-        <v>0.875</v>
-      </c>
-      <c r="H13" s="37">
+        <v>0.9</v>
+      </c>
+      <c r="H13" s="36">
         <f t="shared" si="0"/>
         <v>0.61665999999999999</v>
       </c>
-      <c r="I13" s="63">
+      <c r="I13" s="62">
         <f t="shared" si="0"/>
         <v>0.61680000000000013</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="36">
         <f t="shared" si="0"/>
         <v>0.81665999999999994</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="39">
         <f t="shared" si="0"/>
-        <v>0.52100000000000013</v>
-      </c>
-      <c r="L13" s="36">
+        <v>0.43680000000000013</v>
+      </c>
+      <c r="L13" s="35">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="M13" s="63">
+      <c r="M13" s="62">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O13" s="44">
+      <c r="O13" s="43">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P13" s="36">
+      <c r="P13" s="35">
         <f t="shared" si="0"/>
         <v>0.60314000000000001</v>
       </c>
-      <c r="Q13" s="63">
+      <c r="Q13" s="62">
         <f t="shared" si="0"/>
         <v>0.80017999999999989</v>
       </c>
-      <c r="R13" s="37">
+      <c r="R13" s="36">
         <f t="shared" si="0"/>
         <v>0.60936000000000001</v>
       </c>
-      <c r="S13" s="44">
+      <c r="S13" s="43">
         <f t="shared" si="0"/>
-        <v>0.51090000000000002</v>
-      </c>
-      <c r="T13" s="54">
+        <v>0.60872000000000004</v>
+      </c>
+      <c r="T13" s="53">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
         <v>381</v>
       </c>
-      <c r="U13" s="67">
+      <c r="U13" s="66">
         <f t="shared" si="1"/>
         <v>1243.2</v>
       </c>
-      <c r="V13" s="55">
+      <c r="V13" s="54">
         <f t="shared" si="1"/>
         <v>452.8</v>
       </c>
-      <c r="W13" s="56">
+      <c r="W13" s="55">
         <f t="shared" si="1"/>
-        <v>1747.5</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="E14" s="64" t="s">
+      <c r="E14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="64" t="s">
+      <c r="M14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="64" t="s">
+      <c r="Q14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="U14" s="64" t="s">
+      <c r="U14" s="63" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1904,15 +1913,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="73" t="s">
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
-      <c r="S17" s="73"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1933,17 +1942,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="73" t="s">
+      <c r="M18" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="73">
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72">
         <v>1711</v>
       </c>
-      <c r="Q18" s="73"/>
-      <c r="R18" s="73"/>
-      <c r="S18" s="73"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="72"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -1967,17 +1976,17 @@
       <c r="I19" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="73" t="s">
+      <c r="M19" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="73"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="73">
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72">
         <v>9407</v>
       </c>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="73"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -1998,17 +2007,17 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="M20" s="73" t="s">
+      <c r="M20" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="73"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="77">
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="76">
         <v>1162725581</v>
       </c>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="77"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -2029,17 +2038,17 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="M21" s="74" t="s">
+      <c r="M21" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="78" t="s">
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="78"/>
-      <c r="S21" s="78"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="77"/>
+      <c r="S21" s="77"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
@@ -2099,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="B5:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2115,46 +2124,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="81" t="s">
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="83"/>
-      <c r="M2" s="91" t="s">
+      <c r="K2" s="82"/>
+      <c r="M2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="93"/>
-      <c r="O2" s="81" t="s">
+      <c r="N2" s="92"/>
+      <c r="O2" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="83"/>
+      <c r="P2" s="82"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="89"/>
-      <c r="I3" s="90"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="14" t="s">
         <v>11</v>
       </c>
@@ -2173,7 +2182,7 @@
       <c r="P3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="27" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -2196,7 +2205,7 @@
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="98" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2229,7 +2238,7 @@
       <c r="N4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="94" t="s">
+      <c r="O4" s="93" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="22" t="s">
@@ -2256,13 +2265,13 @@
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="57">
+      <c r="D5" s="56">
         <v>0</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -2277,10 +2286,10 @@
       <c r="I5" s="6">
         <v>0.01</v>
       </c>
-      <c r="J5" s="59">
+      <c r="J5" s="58">
         <v>0</v>
       </c>
-      <c r="K5" s="59">
+      <c r="K5" s="58">
         <v>0</v>
       </c>
       <c r="M5" s="23">
@@ -2289,10 +2298,10 @@
       <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="95">
-        <v>1</v>
-      </c>
-      <c r="P5" s="61">
+      <c r="O5" s="94">
+        <v>1</v>
+      </c>
+      <c r="P5" s="60">
         <v>1</v>
       </c>
     </row>
@@ -2300,7 +2309,7 @@
       <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5">
@@ -2333,10 +2342,10 @@
       <c r="N6" s="24">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="O6" s="95">
-        <v>1</v>
-      </c>
-      <c r="P6" s="61">
+      <c r="O6" s="94">
+        <v>1</v>
+      </c>
+      <c r="P6" s="60">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
@@ -2344,22 +2353,22 @@
       <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="56">
         <v>0</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <v>0</v>
       </c>
       <c r="F7" s="6">
         <v>0.25</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="56">
         <v>0</v>
       </c>
-      <c r="H7" s="58">
+      <c r="H7" s="57">
         <v>0</v>
       </c>
       <c r="I7" s="6">
@@ -2377,10 +2386,10 @@
       <c r="N7" s="24">
         <v>1</v>
       </c>
-      <c r="O7" s="95">
-        <v>1</v>
-      </c>
-      <c r="P7" s="61">
+      <c r="O7" s="94">
+        <v>1</v>
+      </c>
+      <c r="P7" s="60">
         <v>1</v>
       </c>
     </row>
@@ -2388,7 +2397,7 @@
       <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="5">
@@ -2421,10 +2430,10 @@
       <c r="N8" s="24">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="O8" s="95">
-        <v>1</v>
-      </c>
-      <c r="P8" s="61">
+      <c r="O8" s="94">
+        <v>1</v>
+      </c>
+      <c r="P8" s="60">
         <v>1</v>
       </c>
     </row>
@@ -2432,7 +2441,7 @@
       <c r="B9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="5">
@@ -2441,7 +2450,7 @@
       <c r="E9" s="17">
         <v>1</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <v>0</v>
       </c>
       <c r="G9" s="5">
@@ -2450,25 +2459,33 @@
       <c r="H9" s="17">
         <v>0.15</v>
       </c>
-      <c r="I9" s="59">
+      <c r="I9" s="58">
         <v>0</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="58">
         <v>0</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="58">
         <v>0</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="24"/>
+      <c r="M9" s="23">
+        <v>1</v>
+      </c>
+      <c r="N9" s="24">
+        <v>1</v>
+      </c>
+      <c r="O9" s="94">
+        <v>1</v>
+      </c>
+      <c r="P9" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="5"/>
@@ -2481,14 +2498,14 @@
       <c r="K10" s="6"/>
       <c r="M10" s="23"/>
       <c r="N10" s="24"/>
-      <c r="O10" s="95"/>
+      <c r="O10" s="94"/>
       <c r="P10" s="24"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="5"/>
@@ -2501,12 +2518,12 @@
       <c r="K11" s="6"/>
       <c r="M11" s="23"/>
       <c r="N11" s="24"/>
-      <c r="O11" s="95"/>
+      <c r="O11" s="94"/>
       <c r="P11" s="24"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
-      <c r="C12" s="46"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="5"/>
       <c r="E12" s="17"/>
       <c r="F12" s="6"/>
@@ -2517,12 +2534,12 @@
       <c r="K12" s="6"/>
       <c r="M12" s="23"/>
       <c r="N12" s="24"/>
-      <c r="O12" s="95"/>
+      <c r="O12" s="94"/>
       <c r="P12" s="24"/>
     </row>
     <row r="13" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="47"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="9"/>
       <c r="E13" s="18"/>
       <c r="F13" s="10"/>
@@ -2531,9 +2548,9 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="95"/>
       <c r="P13" s="25"/>
     </row>
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2570,18 +2587,20 @@
         <v>0.22589999999999999</v>
       </c>
       <c r="M14" s="26">
-        <f t="shared" ref="M14:N14" si="3">AVERAGE(M5:M13)</f>
-        <v>0.875</v>
-      </c>
-      <c r="N14" s="27">
+        <f t="shared" ref="M14:P14" si="3">AVERAGE(M5:M13)</f>
+        <v>0.9</v>
+      </c>
+      <c r="N14" s="26">
         <f t="shared" si="3"/>
-        <v>0.52100000000000013</v>
+        <v>0.61680000000000013</v>
       </c>
       <c r="O14" s="26">
-        <v>1</v>
-      </c>
-      <c r="P14" s="27">
-        <v>0.63263333333333327</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="26">
+        <f t="shared" si="3"/>
+        <v>0.80017999999999989</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
test 2 - query 2_wn
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2320" yWindow="900" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -837,6 +837,39 @@
     <xf numFmtId="43" fontId="7" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -846,40 +879,13 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -915,12 +921,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,64 +1220,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="80" t="s">
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="67" t="s">
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="69"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="84"/>
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="74" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="70" t="s">
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="74" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="70" t="s">
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -1694,24 +1694,44 @@
       <c r="C9" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="60"/>
+      <c r="D9" s="30">
+        <v>1</v>
+      </c>
+      <c r="E9" s="60">
+        <v>1</v>
+      </c>
       <c r="F9" s="31"/>
       <c r="G9" s="32"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="60"/>
+      <c r="H9" s="30">
+        <v>1</v>
+      </c>
+      <c r="I9" s="60">
+        <v>3.6999999999999998E-2</v>
+      </c>
       <c r="J9" s="31"/>
       <c r="K9" s="32"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="60"/>
+      <c r="L9" s="30">
+        <v>1</v>
+      </c>
+      <c r="M9" s="60">
+        <v>1</v>
+      </c>
       <c r="N9" s="31"/>
       <c r="O9" s="41"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="60"/>
+      <c r="P9" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="60">
+        <v>5.1499999999999997E-2</v>
+      </c>
       <c r="R9" s="31"/>
       <c r="S9" s="41"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="64"/>
+      <c r="T9" s="47">
+        <v>335</v>
+      </c>
+      <c r="U9" s="64">
+        <v>1137</v>
+      </c>
       <c r="V9" s="48"/>
       <c r="W9" s="49"/>
     </row>
@@ -1798,7 +1818,7 @@
       </c>
       <c r="E13" s="62">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
-        <v>0.9</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F13" s="36">
         <f t="shared" si="0"/>
@@ -1810,11 +1830,11 @@
       </c>
       <c r="H13" s="36">
         <f t="shared" si="0"/>
-        <v>0.61665999999999999</v>
+        <v>0.68054999999999988</v>
       </c>
       <c r="I13" s="62">
         <f t="shared" si="0"/>
-        <v>0.61680000000000013</v>
+        <v>0.52016666666666678</v>
       </c>
       <c r="J13" s="36">
         <f t="shared" si="0"/>
@@ -1826,7 +1846,7 @@
       </c>
       <c r="L13" s="35">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M13" s="62">
         <f t="shared" si="0"/>
@@ -1842,11 +1862,11 @@
       </c>
       <c r="P13" s="35">
         <f t="shared" si="0"/>
-        <v>0.60314000000000001</v>
+        <v>0.66928333333333334</v>
       </c>
       <c r="Q13" s="62">
         <f t="shared" si="0"/>
-        <v>0.80017999999999989</v>
+        <v>0.67539999999999989</v>
       </c>
       <c r="R13" s="36">
         <f t="shared" si="0"/>
@@ -1858,11 +1878,11 @@
       </c>
       <c r="T13" s="53">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
-        <v>381</v>
+        <v>373.33333333333331</v>
       </c>
       <c r="U13" s="66">
         <f t="shared" si="1"/>
-        <v>1243.2</v>
+        <v>1225.5</v>
       </c>
       <c r="V13" s="54">
         <f t="shared" si="1"/>
@@ -1891,10 +1911,10 @@
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="78"/>
+      <c r="C17" s="73"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,15 +1933,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72" t="s">
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="72"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="74"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1942,17 +1962,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="72" t="s">
+      <c r="M18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="72">
+      <c r="N18" s="74"/>
+      <c r="O18" s="74"/>
+      <c r="P18" s="74">
         <v>1711</v>
       </c>
-      <c r="Q18" s="72"/>
-      <c r="R18" s="72"/>
-      <c r="S18" s="72"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
+      <c r="S18" s="74"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -1976,17 +1996,17 @@
       <c r="I19" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="72" t="s">
+      <c r="M19" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72">
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74">
         <v>9407</v>
       </c>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="74"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -2007,17 +2027,17 @@
       <c r="H20">
         <v>10</v>
       </c>
-      <c r="M20" s="72" t="s">
+      <c r="M20" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="76">
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="86">
         <v>1162725581</v>
       </c>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
+      <c r="Q20" s="86"/>
+      <c r="R20" s="86"/>
+      <c r="S20" s="86"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -2038,17 +2058,17 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="M21" s="73" t="s">
+      <c r="M21" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="77" t="s">
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
-      <c r="S21" s="77"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="87"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
@@ -2077,14 +2097,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P18:S18"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="M20:O20"/>
@@ -2096,6 +2108,14 @@
     <mergeCell ref="P19:S19"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="M18:O18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P21" r:id="rId1"/>
@@ -2108,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2124,46 +2144,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="83" t="s">
+      <c r="M1" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="80" t="s">
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="82"/>
-      <c r="M2" s="90" t="s">
+      <c r="K2" s="88"/>
+      <c r="M2" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="92"/>
-      <c r="O2" s="80" t="s">
+      <c r="N2" s="98"/>
+      <c r="O2" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="82"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87" t="s">
+      <c r="E3" s="91"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="89"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="95"/>
       <c r="J3" s="14" t="s">
         <v>11</v>
       </c>
@@ -2205,7 +2225,7 @@
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="72" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2238,7 +2258,7 @@
       <c r="N4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="93" t="s">
+      <c r="O4" s="67" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="22" t="s">
@@ -2298,7 +2318,7 @@
       <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="94">
+      <c r="O5" s="68">
         <v>1</v>
       </c>
       <c r="P5" s="60">
@@ -2342,7 +2362,7 @@
       <c r="N6" s="24">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="O6" s="94">
+      <c r="O6" s="68">
         <v>1</v>
       </c>
       <c r="P6" s="60">
@@ -2386,7 +2406,7 @@
       <c r="N7" s="24">
         <v>1</v>
       </c>
-      <c r="O7" s="94">
+      <c r="O7" s="68">
         <v>1</v>
       </c>
       <c r="P7" s="60">
@@ -2430,7 +2450,7 @@
       <c r="N8" s="24">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="O8" s="94">
+      <c r="O8" s="68">
         <v>1</v>
       </c>
       <c r="P8" s="60">
@@ -2474,7 +2494,7 @@
       <c r="N9" s="24">
         <v>1</v>
       </c>
-      <c r="O9" s="94">
+      <c r="O9" s="68">
         <v>1</v>
       </c>
       <c r="P9" s="24">
@@ -2498,7 +2518,7 @@
       <c r="K10" s="6"/>
       <c r="M10" s="23"/>
       <c r="N10" s="24"/>
-      <c r="O10" s="94"/>
+      <c r="O10" s="68"/>
       <c r="P10" s="24"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
@@ -2518,7 +2538,7 @@
       <c r="K11" s="6"/>
       <c r="M11" s="23"/>
       <c r="N11" s="24"/>
-      <c r="O11" s="94"/>
+      <c r="O11" s="68"/>
       <c r="P11" s="24"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
@@ -2534,7 +2554,7 @@
       <c r="K12" s="6"/>
       <c r="M12" s="23"/>
       <c r="N12" s="24"/>
-      <c r="O12" s="94"/>
+      <c r="O12" s="68"/>
       <c r="P12" s="24"/>
     </row>
     <row r="13" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2548,9 +2568,9 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="95"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="71"/>
+      <c r="O13" s="69"/>
       <c r="P13" s="25"/>
     </row>
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test 3 - query 6_wn
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="900" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="920" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -1208,7 +1208,7 @@
   <dimension ref="B1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1700,7 +1700,9 @@
       <c r="E9" s="60">
         <v>1</v>
       </c>
-      <c r="F9" s="31"/>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
       <c r="G9" s="32"/>
       <c r="H9" s="30">
         <v>1</v>
@@ -1708,7 +1710,9 @@
       <c r="I9" s="60">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J9" s="31"/>
+      <c r="J9" s="31">
+        <v>1</v>
+      </c>
       <c r="K9" s="32"/>
       <c r="L9" s="30">
         <v>1</v>
@@ -1716,7 +1720,9 @@
       <c r="M9" s="60">
         <v>1</v>
       </c>
-      <c r="N9" s="31"/>
+      <c r="N9" s="31">
+        <v>1</v>
+      </c>
       <c r="O9" s="41"/>
       <c r="P9" s="30">
         <v>1</v>
@@ -1724,7 +1730,9 @@
       <c r="Q9" s="60">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="R9" s="31"/>
+      <c r="R9" s="31">
+        <v>1</v>
+      </c>
       <c r="S9" s="41"/>
       <c r="T9" s="47">
         <v>335</v>
@@ -1732,7 +1740,9 @@
       <c r="U9" s="64">
         <v>1137</v>
       </c>
-      <c r="V9" s="48"/>
+      <c r="V9" s="48">
+        <v>302</v>
+      </c>
       <c r="W9" s="49"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
@@ -1838,7 +1848,7 @@
       </c>
       <c r="J13" s="36">
         <f t="shared" si="0"/>
-        <v>0.81665999999999994</v>
+        <v>0.84721666666666662</v>
       </c>
       <c r="K13" s="39">
         <f t="shared" si="0"/>
@@ -1870,7 +1880,7 @@
       </c>
       <c r="R13" s="36">
         <f t="shared" si="0"/>
-        <v>0.60936000000000001</v>
+        <v>0.67446666666666666</v>
       </c>
       <c r="S13" s="43">
         <f t="shared" si="0"/>
@@ -1886,7 +1896,7 @@
       </c>
       <c r="V13" s="54">
         <f t="shared" si="1"/>
-        <v>452.8</v>
+        <v>427.66666666666669</v>
       </c>
       <c r="W13" s="55">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
test 4 - query 6_wn
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="920" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="920" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1703,9 @@
       <c r="F9" s="31">
         <v>1</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="32">
+        <v>1</v>
+      </c>
       <c r="H9" s="30">
         <v>1</v>
       </c>
@@ -1713,7 +1715,9 @@
       <c r="J9" s="31">
         <v>1</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="32">
+        <v>3.6999999999999998E-2</v>
+      </c>
       <c r="L9" s="30">
         <v>1</v>
       </c>
@@ -1723,7 +1727,9 @@
       <c r="N9" s="31">
         <v>1</v>
       </c>
-      <c r="O9" s="41"/>
+      <c r="O9" s="41">
+        <v>1</v>
+      </c>
       <c r="P9" s="30">
         <v>1</v>
       </c>
@@ -1733,7 +1739,9 @@
       <c r="R9" s="31">
         <v>1</v>
       </c>
-      <c r="S9" s="41"/>
+      <c r="S9" s="41">
+        <v>5.1499999999999997E-2</v>
+      </c>
       <c r="T9" s="47">
         <v>335</v>
       </c>
@@ -1743,7 +1751,9 @@
       <c r="V9" s="48">
         <v>302</v>
       </c>
-      <c r="W9" s="49"/>
+      <c r="W9" s="49">
+        <v>1555</v>
+      </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -1836,7 +1846,7 @@
       </c>
       <c r="G13" s="36">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="H13" s="36">
         <f t="shared" si="0"/>
@@ -1852,7 +1862,7 @@
       </c>
       <c r="K13" s="39">
         <f t="shared" si="0"/>
-        <v>0.43680000000000013</v>
+        <v>0.37016666666666675</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="0"/>
@@ -1884,7 +1894,7 @@
       </c>
       <c r="S13" s="43">
         <f t="shared" si="0"/>
-        <v>0.60872000000000004</v>
+        <v>0.51585000000000003</v>
       </c>
       <c r="T13" s="53">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
@@ -1900,7 +1910,7 @@
       </c>
       <c r="W13" s="55">
         <f t="shared" si="1"/>
-        <v>2015</v>
+        <v>1938.3333333333333</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
@@ -2138,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2480,8 +2490,8 @@
       <c r="E9" s="17">
         <v>1</v>
       </c>
-      <c r="F9" s="58">
-        <v>0</v>
+      <c r="F9" s="6">
+        <v>1</v>
       </c>
       <c r="G9" s="5">
         <v>0.15</v>
@@ -2489,8 +2499,8 @@
       <c r="H9" s="17">
         <v>0.15</v>
       </c>
-      <c r="I9" s="58">
-        <v>0</v>
+      <c r="I9" s="6">
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="J9" s="58">
         <v>0</v>
@@ -2518,18 +2528,42 @@
       <c r="C10" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="24"/>
+      <c r="D10" s="56">
+        <v>0</v>
+      </c>
+      <c r="E10" s="57">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="56">
+        <v>0</v>
+      </c>
+      <c r="H10" s="57">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="58">
+        <v>0</v>
+      </c>
+      <c r="K10" s="58">
+        <v>0</v>
+      </c>
+      <c r="M10" s="23">
+        <v>1</v>
+      </c>
+      <c r="N10" s="24">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="O10" s="68">
+        <v>1</v>
+      </c>
+      <c r="P10" s="24">
+        <v>5.1499999999999997E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -2586,43 +2620,43 @@
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="11">
         <f>AVERAGE(D5:D13)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>0.65</v>
+        <v>0.875</v>
       </c>
       <c r="G14" s="11">
         <f>AVERAGE(G5:G13)</f>
-        <v>0.14000000000000001</v>
+        <v>0.11666666666666668</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>0.08</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="I14" s="12">
         <f t="shared" si="1"/>
-        <v>0.22059999999999999</v>
+        <v>0.35476666666666667</v>
       </c>
       <c r="J14" s="12">
         <f t="shared" ref="J14:K14" si="2">AVERAGE(J5:J13)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="2"/>
-        <v>0.22589999999999999</v>
+        <v>0.18825</v>
       </c>
       <c r="M14" s="26">
         <f t="shared" ref="M14:P14" si="3">AVERAGE(M5:M13)</f>
-        <v>0.9</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="N14" s="26">
         <f t="shared" si="3"/>
-        <v>0.61680000000000013</v>
+        <v>0.52016666666666678</v>
       </c>
       <c r="O14" s="26">
         <f t="shared" si="3"/>
@@ -2630,7 +2664,7 @@
       </c>
       <c r="P14" s="26">
         <f t="shared" si="3"/>
-        <v>0.80017999999999989</v>
+        <v>0.67539999999999989</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
final execution of word net test
</commit_message>
<xml_diff>
--- a/hammer-colombo/wordnet-examples-set/test.xlsx
+++ b/hammer-colombo/wordnet-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="920" windowWidth="24220" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-420" yWindow="1680" windowWidth="24220" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
   <si>
     <t>th_krm</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Hammer best performance</t>
   </si>
   <si>
-    <t>best test</t>
-  </si>
-  <si>
     <t>execution time [seconds]</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>best</t>
   </si>
   <si>
-    <t>****</t>
-  </si>
-  <si>
     <t>5_wm</t>
   </si>
   <si>
@@ -169,6 +163,18 @@
   </si>
   <si>
     <t>7_wm</t>
+  </si>
+  <si>
+    <t>**** best precision</t>
+  </si>
+  <si>
+    <t>**** good precision and good performance</t>
+  </si>
+  <si>
+    <t>good precision and good performance</t>
+  </si>
+  <si>
+    <t>best test --&gt; 3° test</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +280,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -343,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -675,43 +689,6 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -767,7 +744,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -797,7 +774,6 @@
     <xf numFmtId="10" fontId="7" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -818,13 +794,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="10" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="10" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="10" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="10" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -837,12 +810,9 @@
     <xf numFmtId="43" fontId="7" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="11" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="7" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="7" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,6 +891,13 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1207,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,130 +1197,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="76" t="s">
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="82" t="s">
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="77"/>
+    </row>
+    <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="84"/>
-    </row>
-    <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="72"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="59" t="s">
+      <c r="M3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="29" t="s">
+      <c r="Q3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="29" t="s">
+      <c r="R3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="28" t="s">
+      <c r="T3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="U3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="V3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="40" t="s">
+      <c r="W3" s="39" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1351,67 +1328,67 @@
       <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="30">
-        <v>1</v>
-      </c>
-      <c r="E4" s="60">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31">
-        <v>1</v>
-      </c>
-      <c r="G4" s="31">
-        <v>1</v>
-      </c>
-      <c r="H4" s="56">
+      <c r="D4" s="29">
+        <v>1</v>
+      </c>
+      <c r="E4" s="56">
+        <v>1</v>
+      </c>
+      <c r="F4" s="56">
+        <v>1</v>
+      </c>
+      <c r="G4" s="30">
+        <v>1</v>
+      </c>
+      <c r="H4" s="52">
         <v>0</v>
       </c>
-      <c r="I4" s="60">
-        <v>1</v>
-      </c>
-      <c r="J4" s="31">
-        <v>1</v>
-      </c>
-      <c r="K4" s="32">
-        <v>1</v>
-      </c>
-      <c r="L4" s="56">
+      <c r="I4" s="56">
+        <v>1</v>
+      </c>
+      <c r="J4" s="56">
+        <v>1</v>
+      </c>
+      <c r="K4" s="31">
+        <v>1</v>
+      </c>
+      <c r="L4" s="52">
         <v>0</v>
       </c>
-      <c r="M4" s="60">
-        <v>1</v>
-      </c>
-      <c r="N4" s="31">
-        <v>1</v>
-      </c>
-      <c r="O4" s="41">
-        <v>1</v>
-      </c>
-      <c r="P4" s="56">
+      <c r="M4" s="56">
+        <v>1</v>
+      </c>
+      <c r="N4" s="56">
+        <v>1</v>
+      </c>
+      <c r="O4" s="40">
+        <v>1</v>
+      </c>
+      <c r="P4" s="52">
         <v>0</v>
       </c>
-      <c r="Q4" s="60">
-        <v>1</v>
-      </c>
-      <c r="R4" s="31">
+      <c r="Q4" s="56">
+        <v>1</v>
+      </c>
+      <c r="R4" s="56">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="S4" s="41">
+      <c r="S4" s="40">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="T4" s="47">
+      <c r="T4" s="46">
         <v>211</v>
       </c>
-      <c r="U4" s="64">
+      <c r="U4" s="60">
         <v>479</v>
       </c>
-      <c r="V4" s="48">
+      <c r="V4" s="60">
         <v>448</v>
       </c>
-      <c r="W4" s="49">
+      <c r="W4" s="47">
         <v>475</v>
       </c>
     </row>
@@ -1419,67 +1396,67 @@
       <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="30">
-        <v>1</v>
-      </c>
-      <c r="E5" s="60">
+      <c r="D5" s="29">
+        <v>1</v>
+      </c>
+      <c r="E5" s="56">
         <v>0.5</v>
       </c>
-      <c r="F5" s="31">
-        <v>1</v>
-      </c>
-      <c r="G5" s="32">
+      <c r="F5" s="56">
+        <v>1</v>
+      </c>
+      <c r="G5" s="31">
         <v>0.5</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="I5" s="60">
+      <c r="I5" s="56">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="56">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="31">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="L5" s="30">
-        <v>1</v>
-      </c>
-      <c r="M5" s="60">
-        <v>1</v>
-      </c>
-      <c r="N5" s="31">
-        <v>1</v>
-      </c>
-      <c r="O5" s="41">
-        <v>1</v>
-      </c>
-      <c r="P5" s="30">
+      <c r="L5" s="29">
+        <v>1</v>
+      </c>
+      <c r="M5" s="56">
+        <v>1</v>
+      </c>
+      <c r="N5" s="56">
+        <v>1</v>
+      </c>
+      <c r="O5" s="40">
+        <v>1</v>
+      </c>
+      <c r="P5" s="29">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="Q5" s="60">
+      <c r="Q5" s="56">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="56">
         <v>3.3E-3</v>
       </c>
-      <c r="S5" s="41">
+      <c r="S5" s="40">
         <v>1E-4</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="46">
         <v>627</v>
       </c>
-      <c r="U5" s="64">
+      <c r="U5" s="60">
         <v>3702</v>
       </c>
-      <c r="V5" s="48">
+      <c r="V5" s="60">
         <v>704</v>
       </c>
-      <c r="W5" s="49">
+      <c r="W5" s="47">
         <v>5129</v>
       </c>
     </row>
@@ -1487,67 +1464,67 @@
       <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="30">
-        <v>1</v>
-      </c>
-      <c r="E6" s="60">
-        <v>1</v>
-      </c>
-      <c r="F6" s="31">
-        <v>1</v>
-      </c>
-      <c r="G6" s="32">
-        <v>1</v>
-      </c>
-      <c r="H6" s="30">
-        <v>1</v>
-      </c>
-      <c r="I6" s="60">
-        <v>1</v>
-      </c>
-      <c r="J6" s="31">
-        <v>1</v>
-      </c>
-      <c r="K6" s="32">
-        <v>1</v>
-      </c>
-      <c r="L6" s="30">
-        <v>1</v>
-      </c>
-      <c r="M6" s="60">
-        <v>1</v>
-      </c>
-      <c r="N6" s="31">
-        <v>1</v>
-      </c>
-      <c r="O6" s="41">
-        <v>1</v>
-      </c>
-      <c r="P6" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="60">
-        <v>1</v>
-      </c>
-      <c r="R6" s="31">
-        <v>1</v>
-      </c>
-      <c r="S6" s="41">
-        <v>1</v>
-      </c>
-      <c r="T6" s="47">
+      <c r="D6" s="29">
+        <v>1</v>
+      </c>
+      <c r="E6" s="56">
+        <v>1</v>
+      </c>
+      <c r="F6" s="56">
+        <v>1</v>
+      </c>
+      <c r="G6" s="31">
+        <v>1</v>
+      </c>
+      <c r="H6" s="29">
+        <v>1</v>
+      </c>
+      <c r="I6" s="56">
+        <v>1</v>
+      </c>
+      <c r="J6" s="56">
+        <v>1</v>
+      </c>
+      <c r="K6" s="31">
+        <v>1</v>
+      </c>
+      <c r="L6" s="29">
+        <v>1</v>
+      </c>
+      <c r="M6" s="56">
+        <v>1</v>
+      </c>
+      <c r="N6" s="56">
+        <v>1</v>
+      </c>
+      <c r="O6" s="40">
+        <v>1</v>
+      </c>
+      <c r="P6" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="56">
+        <v>1</v>
+      </c>
+      <c r="R6" s="56">
+        <v>1</v>
+      </c>
+      <c r="S6" s="40">
+        <v>1</v>
+      </c>
+      <c r="T6" s="46">
         <v>499</v>
       </c>
-      <c r="U6" s="64">
+      <c r="U6" s="60">
         <v>705</v>
       </c>
-      <c r="V6" s="48">
+      <c r="V6" s="60">
         <v>465</v>
       </c>
-      <c r="W6" s="49">
+      <c r="W6" s="47">
         <v>507</v>
       </c>
     </row>
@@ -1555,386 +1532,441 @@
       <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="30">
-        <v>1</v>
-      </c>
-      <c r="E7" s="60">
-        <v>1</v>
-      </c>
-      <c r="F7" s="31">
-        <v>1</v>
-      </c>
-      <c r="G7" s="31">
-        <v>1</v>
-      </c>
-      <c r="H7" s="30">
-        <v>1</v>
-      </c>
-      <c r="I7" s="60">
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56">
+        <v>1</v>
+      </c>
+      <c r="F7" s="56">
+        <v>1</v>
+      </c>
+      <c r="G7" s="30">
+        <v>1</v>
+      </c>
+      <c r="H7" s="29">
+        <v>1</v>
+      </c>
+      <c r="I7" s="56">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J7" s="31">
-        <v>1</v>
-      </c>
-      <c r="K7" s="31">
+      <c r="J7" s="56">
+        <v>1</v>
+      </c>
+      <c r="K7" s="30">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="L7" s="30">
-        <v>1</v>
-      </c>
-      <c r="M7" s="60">
-        <v>1</v>
-      </c>
-      <c r="N7" s="31">
-        <v>1</v>
-      </c>
-      <c r="O7" s="31">
-        <v>1</v>
-      </c>
-      <c r="P7" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="60">
-        <v>1</v>
-      </c>
-      <c r="R7" s="31">
-        <v>1</v>
-      </c>
-      <c r="S7" s="31">
-        <v>1</v>
-      </c>
-      <c r="T7" s="47">
+      <c r="L7" s="29">
+        <v>1</v>
+      </c>
+      <c r="M7" s="56">
+        <v>1</v>
+      </c>
+      <c r="N7" s="56">
+        <v>1</v>
+      </c>
+      <c r="O7" s="30">
+        <v>1</v>
+      </c>
+      <c r="P7" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="56">
+        <v>1</v>
+      </c>
+      <c r="R7" s="56">
+        <v>1</v>
+      </c>
+      <c r="S7" s="30">
+        <v>1</v>
+      </c>
+      <c r="T7" s="46">
         <v>260</v>
       </c>
-      <c r="U7" s="64">
+      <c r="U7" s="60">
         <v>987</v>
       </c>
-      <c r="V7" s="48">
+      <c r="V7" s="60">
         <v>300</v>
       </c>
-      <c r="W7" s="49">
+      <c r="W7" s="47">
         <v>879</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="30">
-        <v>1</v>
-      </c>
-      <c r="E8" s="60">
-        <v>1</v>
-      </c>
-      <c r="F8" s="31">
-        <v>1</v>
-      </c>
-      <c r="G8" s="32">
-        <v>1</v>
-      </c>
-      <c r="H8" s="30">
-        <v>1</v>
-      </c>
-      <c r="I8" s="60">
-        <v>1</v>
-      </c>
-      <c r="J8" s="31">
-        <v>1</v>
-      </c>
-      <c r="K8" s="32">
+      <c r="D8" s="29">
+        <v>1</v>
+      </c>
+      <c r="E8" s="56">
+        <v>1</v>
+      </c>
+      <c r="F8" s="56">
+        <v>1</v>
+      </c>
+      <c r="G8" s="31">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29">
+        <v>1</v>
+      </c>
+      <c r="I8" s="56">
+        <v>1</v>
+      </c>
+      <c r="J8" s="56">
+        <v>1</v>
+      </c>
+      <c r="K8" s="31">
         <v>0.1</v>
       </c>
-      <c r="L8" s="30">
-        <v>1</v>
-      </c>
-      <c r="M8" s="60">
-        <v>1</v>
-      </c>
-      <c r="N8" s="31">
-        <v>1</v>
-      </c>
-      <c r="O8" s="41">
-        <v>1</v>
-      </c>
-      <c r="P8" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="60">
-        <v>1</v>
-      </c>
-      <c r="R8" s="31">
-        <v>1</v>
-      </c>
-      <c r="S8" s="41">
-        <v>1</v>
-      </c>
-      <c r="T8" s="47">
+      <c r="L8" s="29">
+        <v>1</v>
+      </c>
+      <c r="M8" s="56">
+        <v>1</v>
+      </c>
+      <c r="N8" s="56">
+        <v>1</v>
+      </c>
+      <c r="O8" s="40">
+        <v>1</v>
+      </c>
+      <c r="P8" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="56">
+        <v>1</v>
+      </c>
+      <c r="R8" s="56">
+        <v>1</v>
+      </c>
+      <c r="S8" s="40">
+        <v>1</v>
+      </c>
+      <c r="T8" s="46">
         <v>308</v>
       </c>
-      <c r="U8" s="64">
+      <c r="U8" s="60">
         <v>343</v>
       </c>
-      <c r="V8" s="48">
+      <c r="V8" s="60">
         <v>347</v>
       </c>
-      <c r="W8" s="49">
+      <c r="W8" s="47">
         <v>3085</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="30">
-        <v>1</v>
-      </c>
-      <c r="E9" s="60">
-        <v>1</v>
-      </c>
-      <c r="F9" s="31">
-        <v>1</v>
-      </c>
-      <c r="G9" s="32">
-        <v>1</v>
-      </c>
-      <c r="H9" s="30">
-        <v>1</v>
-      </c>
-      <c r="I9" s="60">
+      <c r="D9" s="29">
+        <v>1</v>
+      </c>
+      <c r="E9" s="56">
+        <v>1</v>
+      </c>
+      <c r="F9" s="56">
+        <v>1</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1</v>
+      </c>
+      <c r="H9" s="29">
+        <v>1</v>
+      </c>
+      <c r="I9" s="56">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J9" s="31">
-        <v>1</v>
-      </c>
-      <c r="K9" s="32">
+      <c r="J9" s="56">
+        <v>1</v>
+      </c>
+      <c r="K9" s="31">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="L9" s="30">
-        <v>1</v>
-      </c>
-      <c r="M9" s="60">
-        <v>1</v>
-      </c>
-      <c r="N9" s="31">
-        <v>1</v>
-      </c>
-      <c r="O9" s="41">
-        <v>1</v>
-      </c>
-      <c r="P9" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="60">
+      <c r="L9" s="29">
+        <v>1</v>
+      </c>
+      <c r="M9" s="56">
+        <v>1</v>
+      </c>
+      <c r="N9" s="56">
+        <v>1</v>
+      </c>
+      <c r="O9" s="40">
+        <v>1</v>
+      </c>
+      <c r="P9" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="56">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="R9" s="31">
-        <v>1</v>
-      </c>
-      <c r="S9" s="41">
+      <c r="R9" s="56">
+        <v>1</v>
+      </c>
+      <c r="S9" s="40">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="T9" s="47">
+      <c r="T9" s="46">
         <v>335</v>
       </c>
-      <c r="U9" s="64">
+      <c r="U9" s="60">
         <v>1137</v>
       </c>
-      <c r="V9" s="48">
+      <c r="V9" s="60">
         <v>302</v>
       </c>
-      <c r="W9" s="49">
+      <c r="W9" s="47">
         <v>1555</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="49"/>
+      <c r="D10" s="29">
+        <v>1</v>
+      </c>
+      <c r="E10" s="56">
+        <v>1</v>
+      </c>
+      <c r="F10" s="56">
+        <v>1</v>
+      </c>
+      <c r="G10" s="40">
+        <v>1</v>
+      </c>
+      <c r="H10" s="29">
+        <v>1</v>
+      </c>
+      <c r="I10" s="56">
+        <v>1</v>
+      </c>
+      <c r="J10" s="56">
+        <v>1</v>
+      </c>
+      <c r="K10" s="40">
+        <v>1</v>
+      </c>
+      <c r="L10" s="29">
+        <v>1</v>
+      </c>
+      <c r="M10" s="56">
+        <v>1</v>
+      </c>
+      <c r="N10" s="56">
+        <v>1</v>
+      </c>
+      <c r="O10" s="40">
+        <v>1</v>
+      </c>
+      <c r="P10" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="56">
+        <v>1</v>
+      </c>
+      <c r="R10" s="56">
+        <v>1</v>
+      </c>
+      <c r="S10" s="40">
+        <v>1</v>
+      </c>
+      <c r="T10" s="46">
+        <v>297</v>
+      </c>
+      <c r="U10" s="60">
+        <v>423</v>
+      </c>
+      <c r="V10" s="60">
+        <v>347</v>
+      </c>
+      <c r="W10" s="47">
+        <v>274</v>
+      </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="49"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="47"/>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="65"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="52"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="61"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="49"/>
     </row>
     <row r="13" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <f>AVERAGE(D4:D12)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E13" s="58">
         <f t="shared" ref="E13:S13" si="0">AVERAGE(E4:E12)</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F13" s="36">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F13" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <f t="shared" si="0"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="H13" s="36">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="H13" s="35">
         <f t="shared" si="0"/>
-        <v>0.68054999999999988</v>
-      </c>
-      <c r="I13" s="62">
+        <v>0.72618571428571421</v>
+      </c>
+      <c r="I13" s="58">
         <f t="shared" si="0"/>
-        <v>0.52016666666666678</v>
-      </c>
-      <c r="J13" s="36">
+        <v>0.58871428571428575</v>
+      </c>
+      <c r="J13" s="58">
         <f t="shared" si="0"/>
-        <v>0.84721666666666662</v>
-      </c>
-      <c r="K13" s="39">
+        <v>0.86904285714285712</v>
+      </c>
+      <c r="K13" s="38">
         <f t="shared" si="0"/>
-        <v>0.37016666666666675</v>
-      </c>
-      <c r="L13" s="35">
+        <v>0.46014285714285724</v>
+      </c>
+      <c r="L13" s="34">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="M13" s="62">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M13" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N13" s="36">
+      <c r="N13" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="42">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P13" s="35">
+      <c r="P13" s="34">
         <f t="shared" si="0"/>
-        <v>0.66928333333333334</v>
-      </c>
-      <c r="Q13" s="62">
+        <v>0.7165285714285714</v>
+      </c>
+      <c r="Q13" s="58">
         <f t="shared" si="0"/>
-        <v>0.67539999999999989</v>
-      </c>
-      <c r="R13" s="36">
+        <v>0.72177142857142851</v>
+      </c>
+      <c r="R13" s="58">
         <f t="shared" si="0"/>
-        <v>0.67446666666666666</v>
-      </c>
-      <c r="S13" s="43">
+        <v>0.7209714285714286</v>
+      </c>
+      <c r="S13" s="42">
         <f t="shared" si="0"/>
-        <v>0.51585000000000003</v>
-      </c>
-      <c r="T13" s="53">
+        <v>0.58501428571428582</v>
+      </c>
+      <c r="T13" s="50">
         <f t="shared" ref="T13:W13" si="1">AVERAGE(T4:T12)</f>
-        <v>373.33333333333331</v>
-      </c>
-      <c r="U13" s="66">
+        <v>362.42857142857144</v>
+      </c>
+      <c r="U13" s="62">
         <f t="shared" si="1"/>
-        <v>1225.5</v>
-      </c>
-      <c r="V13" s="54">
+        <v>1110.8571428571429</v>
+      </c>
+      <c r="V13" s="62">
         <f t="shared" si="1"/>
-        <v>427.66666666666669</v>
-      </c>
-      <c r="W13" s="55">
+        <v>416.14285714285717</v>
+      </c>
+      <c r="W13" s="51">
         <f t="shared" si="1"/>
-        <v>1938.3333333333333</v>
+        <v>1700.5714285714287</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="E14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="U14" s="63" t="s">
-        <v>42</v>
+      <c r="E14" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="V14" s="59" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="73"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1953,15 +1985,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74" t="s">
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="67"/>
+      <c r="S17" s="67"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1982,17 +2014,17 @@
       <c r="H18">
         <v>10</v>
       </c>
-      <c r="M18" s="74" t="s">
+      <c r="M18" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="74"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74">
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67">
         <v>1711</v>
       </c>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="74"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="67"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -2014,50 +2046,57 @@
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>43</v>
-      </c>
-      <c r="M19" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="74"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="74">
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67">
         <v>9407</v>
       </c>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74"/>
-      <c r="S19" s="74"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="92"/>
+      <c r="D20" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="92">
         <v>3</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="92">
         <v>10</v>
       </c>
-      <c r="M20" s="74" t="s">
+      <c r="I20" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="86">
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="79">
         <v>1162725581</v>
       </c>
-      <c r="Q20" s="86"/>
-      <c r="R20" s="86"/>
-      <c r="S20" s="86"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -2078,17 +2117,17 @@
       <c r="H21">
         <v>10</v>
       </c>
-      <c r="M21" s="85" t="s">
+      <c r="M21" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="85"/>
-      <c r="O21" s="85"/>
-      <c r="P21" s="87" t="s">
+      <c r="N21" s="78"/>
+      <c r="O21" s="78"/>
+      <c r="P21" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="Q21" s="87"/>
-      <c r="R21" s="87"/>
-      <c r="S21" s="87"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
@@ -2148,62 +2187,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
     </row>
     <row r="2" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="76" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="88"/>
-      <c r="M2" s="96" t="s">
+      <c r="K2" s="81"/>
+      <c r="M2" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="76" t="s">
+      <c r="N2" s="91"/>
+      <c r="O2" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="88"/>
+      <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93" t="s">
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="88"/>
       <c r="J3" s="14" t="s">
         <v>11</v>
       </c>
@@ -2222,8 +2264,8 @@
       <c r="P3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="27" t="s">
-        <v>39</v>
+      <c r="Q3" s="94" t="s">
+        <v>48</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>0</v>
@@ -2245,7 +2287,7 @@
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2278,26 +2320,26 @@
       <c r="N4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="67" t="s">
+      <c r="O4" s="21" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="2"/>
-      <c r="R4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" t="s">
-        <v>4</v>
-      </c>
-      <c r="U4">
+      <c r="R4" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="92">
         <v>3</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="92">
         <v>10</v>
       </c>
     </row>
@@ -2305,13 +2347,13 @@
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="52">
         <v>0</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="53">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -2326,10 +2368,10 @@
       <c r="I5" s="6">
         <v>0.01</v>
       </c>
-      <c r="J5" s="58">
+      <c r="J5" s="54">
         <v>0</v>
       </c>
-      <c r="K5" s="58">
+      <c r="K5" s="54">
         <v>0</v>
       </c>
       <c r="M5" s="23">
@@ -2338,18 +2380,18 @@
       <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="68">
-        <v>1</v>
-      </c>
-      <c r="P5" s="60">
-        <v>1</v>
+      <c r="O5" s="23">
+        <v>1</v>
+      </c>
+      <c r="P5" s="24">
+        <v>4.3499999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5">
@@ -2377,38 +2419,38 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="M6" s="23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N6" s="24">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="O6" s="68">
-        <v>1</v>
-      </c>
-      <c r="P6" s="60">
-        <v>8.9999999999999998E-4</v>
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="O6" s="23">
+        <v>1</v>
+      </c>
+      <c r="P6" s="24">
+        <v>3.3E-3</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="52">
         <v>0</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="53">
         <v>0</v>
       </c>
       <c r="F7" s="6">
         <v>0.25</v>
       </c>
-      <c r="G7" s="56">
+      <c r="G7" s="52">
         <v>0</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="53">
         <v>0</v>
       </c>
       <c r="I7" s="6">
@@ -2426,10 +2468,10 @@
       <c r="N7" s="24">
         <v>1</v>
       </c>
-      <c r="O7" s="68">
-        <v>1</v>
-      </c>
-      <c r="P7" s="60">
+      <c r="O7" s="23">
+        <v>1</v>
+      </c>
+      <c r="P7" s="24">
         <v>1</v>
       </c>
     </row>
@@ -2437,7 +2479,7 @@
       <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="5">
@@ -2468,20 +2510,20 @@
         <v>1</v>
       </c>
       <c r="N8" s="24">
-        <v>7.6899999999999996E-2</v>
-      </c>
-      <c r="O8" s="68">
-        <v>1</v>
-      </c>
-      <c r="P8" s="60">
+        <v>1</v>
+      </c>
+      <c r="O8" s="23">
+        <v>1</v>
+      </c>
+      <c r="P8" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="5">
@@ -2502,10 +2544,10 @@
       <c r="I9" s="6">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="54">
         <v>0</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="54">
         <v>0</v>
       </c>
       <c r="M9" s="23">
@@ -2514,7 +2556,7 @@
       <c r="N9" s="24">
         <v>1</v>
       </c>
-      <c r="O9" s="68">
+      <c r="O9" s="23">
         <v>1</v>
       </c>
       <c r="P9" s="24">
@@ -2523,71 +2565,95 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="52">
         <v>0</v>
       </c>
-      <c r="E10" s="57">
+      <c r="E10" s="53">
         <v>0</v>
       </c>
       <c r="F10" s="6">
         <v>1</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="52">
         <v>0</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="53">
         <v>0</v>
       </c>
       <c r="I10" s="6">
         <v>1</v>
       </c>
-      <c r="J10" s="58">
+      <c r="J10" s="54">
         <v>0</v>
       </c>
-      <c r="K10" s="58">
+      <c r="K10" s="54">
         <v>0</v>
       </c>
       <c r="M10" s="23">
         <v>1</v>
       </c>
       <c r="N10" s="24">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="O10" s="68">
+        <v>1</v>
+      </c>
+      <c r="O10" s="23">
         <v>1</v>
       </c>
       <c r="P10" s="24">
-        <v>5.1499999999999997E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="24"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="23">
+        <v>1</v>
+      </c>
+      <c r="N11" s="24">
+        <v>1</v>
+      </c>
+      <c r="O11" s="23">
+        <v>1</v>
+      </c>
+      <c r="P11" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
-      <c r="C12" s="45"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="5"/>
       <c r="E12" s="17"/>
       <c r="F12" s="6"/>
@@ -2598,12 +2664,12 @@
       <c r="K12" s="6"/>
       <c r="M12" s="23"/>
       <c r="N12" s="24"/>
-      <c r="O12" s="68"/>
+      <c r="O12" s="23"/>
       <c r="P12" s="24"/>
     </row>
     <row r="13" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="46"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="9"/>
       <c r="E13" s="18"/>
       <c r="F13" s="10"/>
@@ -2612,59 +2678,59 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="69"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="96"/>
       <c r="P13" s="25"/>
     </row>
     <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="11">
         <f>AVERAGE(D5:D13)</f>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>0.875</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="G14" s="11">
         <f>AVERAGE(G5:G13)</f>
-        <v>0.11666666666666668</v>
+        <v>0.24285714285714288</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>6.6666666666666666E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="I14" s="12">
         <f t="shared" si="1"/>
-        <v>0.35476666666666667</v>
+        <v>0.44694285714285714</v>
       </c>
       <c r="J14" s="12">
         <f t="shared" ref="J14:K14" si="2">AVERAGE(J5:J13)</f>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="2"/>
-        <v>0.18825</v>
+        <v>0.30421428571428571</v>
       </c>
       <c r="M14" s="26">
         <f t="shared" ref="M14:P14" si="3">AVERAGE(M5:M13)</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="N14" s="26">
+        <v>1</v>
+      </c>
+      <c r="N14" s="95">
         <f t="shared" si="3"/>
-        <v>0.52016666666666678</v>
+        <v>0.86904285714285712</v>
       </c>
       <c r="O14" s="26">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="95">
         <f t="shared" si="3"/>
-        <v>0.67539999999999989</v>
+        <v>0.7209714285714286</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">

</xml_diff>